<commit_message>
changed the matching conditon of star rank.
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125">
   <si>
     <t>Product Name</t>
   </si>
@@ -42,10 +42,355 @@
     <t>4.5 out of 5 stars</t>
   </si>
   <si>
-    <t>29,473 customer reviews</t>
+    <t>29,480 customer reviews</t>
   </si>
   <si>
     <t>Twin:$24.95/Twin XL:$24.95/Full:$25.95/Queen:$26.95/King:$34.95/California King:$34.95</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71vbQ0hLE1L._SX450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_garden_sr_pg1_1?ie=UTF8&amp;adId=A2RW43F66B4DM6&amp;url=https%3A%2F%2Fwww.amazon.com%2FSafeRest-Hypoallergenic-Waterproof-Mattress-Protector%2Fdp%2FB003PWNH4Q%2Fref%3Dsr_1_1_sspa%3Fs%3Dbedbath%26ie%3DUTF8%26qid%3D1522624327%26sr%3D1-1-spons%26keywords%3Dmattress%2Bprotector%26psc%3D1&amp;qualifier=1522624327&amp;id=3898230458598911&amp;widgetName=sp_atf</t>
+  </si>
+  <si>
+    <t>[Sponsored]LINENSPA Premium Smooth Fabric Mattress Protector - 100% Waterproof - Hypoallergenic - 10 Year Warranty - Vinyl Free - Queen</t>
+  </si>
+  <si>
+    <t>4.2 out of 5 stars</t>
+  </si>
+  <si>
+    <t>6,067 customer reviews</t>
+  </si>
+  <si>
+    <t>Full XL:$19.99/Twin XL:$16.99/California King:$19.99/Full:$16.99/King:$18.99/King Pillow Protector:$9.99/Queen:$15.99/Queen Pillow Protector:$9.99/Standard Pillow Protector:$8.99/Twin:$14.99</t>
+  </si>
+  <si>
+    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDAAoHBwgHBgoICAgLCgoLDhgQDg0NDh0VFhEYIx8lJCIfIiEmKzcvJik0KSEiMEExNDk7Pj4+JS5ESUM8SDc9Pjv/2wBDAQoLCw4NDhwQEBw7KCIoOzs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozv/wAARCAEsASwDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD2WiiigAooooAKKKKACio450lzgEAHgkdakyD0NABRRRQAUUUUAFFFFABRRRQAUUUUAFFFFABRRRQAUUUUAFFFFABRRRQAUUUUAFFFFABRRRQAUUUUAFFFFABRRRQAUUUUAFQSuHJT+AfePrT5GYsI1yM9WHaud1nxHbxm50/TbqC41KCJ5FgjcO+UwWUr2PI6+vAODQBtKW80DeMcg89Kr20znfz8rc4NVbC7t7+2+22sgkikVgXX+9ggr68HipbIYIBPGwUAXlJyPmIH1qQOw/iNQDj6VKp6CmA/zWHvTvNI6gfnUfU0GgCUSg/wmlEin1/Koe1JSAsb1/vClqueD1NH4UAWMUVX3EdzTvMYdyaAJqKi809/5Uvm+woAkopglHoaXev+RQA6ik3L/eFLQAUUUUAFFFFABRRRQAUUUUAFFFFABRRRQAUUUUAFFFFABRRRQBheKblYdHmMpkEHmRLP5X3mjLqGUfUZHHPJritF09b/AFi91jSLkPbfaiZjeOZWEZQ7fKAAC53ycHjkeldH47kx4Q1O4bACPEQT7SriuU+HOqQs81hFlmmjBbZj5EVzlz7ZcjI74+tLqB6Alvb2dl5EMaQoi5EUYAVM+w96LFXCxLKwaRYV3MBgE96A0eDDDEFjxg+/XueTT7VP3rgdNgA/DNMCyDjipF6VEeT709Dt+vSmBJRS7WHPBpMH0oASlow2OhoNABSfhRnPOaXtQAZ9aOvSjt1pPbNABS4pKAeaAFxQKDQPSgAyfWjJ9BRj0oIJHvQA7d6E/nS729TUYNOz6UAPEh9R+VL5hzjAqMHApCRjnmgCXzB6UvmD0NRD3pcgUgJd6+tG5fWot4+tJvNAEwZT0I/OlqD5T0H4VEJMS4DfJ15FAFyikX7o5J+tLQAUUUUAFFFFABRRRQBz3ibTk1LSpbBoTOjzRSToOR5SyKzA+uQCMDk5/Go3tv7Q1bTWtYHENhI8kty8ZTcGiKiMAgbsllY4G1dgHXgbjqXlJZQERtyj+8fU06UsUIzgn0oAzcbYG5LPuPQdT7ChS6ToSDjZ19D7irG9oD5g+gqONcy9c7hnnr1oAk3EnPelkcAZ9BSsuCQKjkABHHBI5piL56mihupqOaZIIjI/0AHc1LaSuxjxS1hTarcPllIVBnkHav4Hqf8APSo7fV7gncCSo5PO7A9+/auF5hRUrHSsLUtc6AqOuBSbF64/KobS7ju49y43AZIB6+4qeu6MlJXWxztNOzG+WOxNHl/7VOoPWqEM2N7Um1vSpKKAI+fQ0uaf2oz+NADN3vSZp+1T/CKVYwc5B9qAIzwc/nRT/J9zTfKI/j/SgBM5oFLscelJhv7poATOG9u1B6Uh9CCKUHtQACndsU3PpS9aADHpUc6r56Oeu2pM0yRA8q5OAFNAFwfdFFIv3B9KWkAUUUUAFFFFABRRRQBE4yTzTeQhzzUjfeNRue3agCpdtttlOD8zgVFGv+m53dEHHtzVi6J8ldoB+bqe1VYx/pgPbyxzQBbbliCcD1pJOVCH1FNJ/eE+2KR2J2Z/vD+dMRePWsnV3Z544ASBkLwPxPT2/lWsevSsbV1YXiMCgJxy/wB0AjH864sa2qOh0Yf4xIYoYNP/ALRuLczLx5MXGI0JwDg9SeCTyas3sen3ExtXiMcmQvmoMbWYEge/T6dKQhrzw/HDGyJJ8qNvOArKRkfpRLZvNfrIrLskljmJ3DjaDkY/KudQ91RjG6aX6/8AA9DVy95tuzV/0/4JQgeWyu8sMMr7XCjjd1/8eHNdAcHkcg1hajsbVZGQfOHRN3PBxk+3TFbUB/0aLHTYP5VpgvdlOmtkTiNVGXVj6OtJQa9E5Bf5UlG4Um7mgBaWk75rK8QeJbDw1aefevh3B8tAOtAyr4n8YWnhzbAFE966lvLz8saju39B39q4e7+IWsSSBTeLAGPKxoBtH1P/ANeuRefUPFHiK7mtwZZJmyWPCj1Jz0Aq0raNoMjC9b+07s8HbxGh789TWLuzeKSRsS+PdXkl/dahPFEv3SSMH8SMmuw8K/EOx1SWLTdTuFjvXIWKXACzH09m/IHtXl11PZXhMkGW3ciMHaR9PX9KpxMg3KXcsT0PVfwPWhKw2lLQ+kTkHBo71yngDxOdc0z7HdOGu7ZeHB/1iDjP1HAP4V1TMqDLVakmrmLi07Ds8ZPSq8045Ax9ajmuCapzT7QWY4FZTqdjWFLuSNdSCRUR+W9qkSeYybQFK57iqGnt5yveN0b5Y/p61oWoy2fas4yk+prOMUti1TWwXyTjjilU8UNxIARng12M4yyv3B9KWkX7i/SlpAFFFFABRRRQAUUUUAMc/NULY5JFPkPznHWkblRxzQBXnBMQUd2FVoh/pQ/3B/WrsxAgwSAWIANU0BW5UeiYzQBMV+YmkbAeMdi4/nSv8r55poI86MHu4/nTEaJHNVNRtPtVv8o+ZfTqRVw9aPeonBTi4vqVGTi7o5iC7lspWOEKkDfG/wB2QjuD2OB75NWH1kOA1vaLFIBjzJGGEyPTv9OO1atxp9vcksQVY9SO9Vl0SENksoA6bUwR+teX9XxMPdhLQ7Pa0ZayWpm2sDXMwC7ioJIdvvMT1c/0HbpW3ukB+5gdgKlht4rdNsYxnqe5p74RC7dFGa7cPRVGLvuznq1PaMrl9o3N8q+pqCbUUhGQhI/vEZH/ANao2lMkhdiTnpt5/U8Cs6/1mXT50Bt5VGepGQ3tTlVb20HGmaVrq1vd71UgtH94dxVlZUdFdTlW6e1ctJeBNQjvUwscoKuAOoq9p14ysYZjiJz8p9CehqYVmnZlyo6XRtyTrFEWz+FcJ8TtFm1vSLS9RtrWjEyLjOUP/wCqu0VPs9nLeXOJQil1A6EAZrMnnMkrHhkbgqehFXOb0YqcE2zxW51uOy0v+zdJPlDOZHHWT/61YTyGUlzkgjmtfxroo0LxLNBCu22mImg/2FJ6fgcj8qyYxvbsMnH41otVcTVnYfFG8WJAeOtW2ufMA80DcOjj+tQLIArIRuU9VP8ASgfJ8rEmMnhj1H1p2A6bwrqsmj6tBqETExhwJVz69T+Ir2qa6SQiRHDI4DKR3B5FeAWKyW0it/yzPB56Z7/SvYfBeox6poIsmtmE1mSjSSLtDrk4K+vA+mc1hJa2NPOxrM+T1rG1OdrucadE+13GWI6ha1r+3ntoTJaxyXJ6GNRlh6Vm6RpN7G0uoXlrItxKehH3R2FYTUr2sbQcbc1zVVFiiSFBhUUACr9mvDN7VnROGPoR2rUtuLc+9bUleRjV0iKtIT+8H0NC9PrQ+dwxzxXWchaX7g+lLSD7o+lLSAKKKKACiiigAooooAhkGZT60gPTNKy/O59aYo5yTQBFfoHtGU9CRUC8Sx5/uYqe8+aDA/vDOagY4mix/dNAD2zk0i4EsfGfmFI33jQh/wBIiH+0KYjSyM0uaD1opDDNGaKOPSgA4PSqWqXUNrbr5p+8eF/vH0q5gVlasNzj91HI8fKGTjZnuD2rKs2oaGlNXlqczrWuSoDE8RlLH7kfX6YIIIrNt5NRKbl8y3Vj9wnj8s1s3MVvAn226ZrgRcIo+6zegHf6n8qgglluJTPOArn7qD+EfWuBPud6j2LaWEcUW4u0rHnLHv7Co5roWsJWQZUcg+lWYlJGCar35gQxxyljJMSI4kXc7Y6kAdverktLoI2ejJ4dWe+0SeGB1bfA4ibPGcdD6VHZzfarSKbYULoGZD1QkdK5HUDNol2qwrIovH2CDGCXPTH16Yrf1Zriwt/tVndeTJbgFwy7o5B3DL/UEHNEJN7lSpqKuupg/ErSXvtNgvIl3S25IOO6nqP0ry+HqVPGemfX0Ne7Qyi/tTDfRJG0q8BG3LJ7qT0I9D+tee+KPAGoWckl/pcX2uAnc8cf3h7gV0QlbRmE4X16nI7t5GQdw496mhBDfMoZTwfemxRCQbySpXjdj07H0NW1aJlC5UFu45BNaORmkXYgtpCZS+YY13HPPHp717Voo26JpXyCMi1UBR2GBxXlHhTw/L4ivvs7q39nWb75n7SOOiD8eTXsMMyLEqMOV4CqOgrPrqVJaWJnuHhUMhAJxnP41atrtbkYHDjt2NYF/qsLXC2EHzyqcyEdE9vrzVy0YqVIPIPFKNX3rLYUqPuXe5p3Nolyu4fLKBw3+NLHFttwGHzKOfrUwIYAjuKa+dpx0xXRyq9zm5naxCOlI2d6/Q0ZpG/1q844NWSXB90UUdhRSAKKKKACiiigAooooAilAzUJOOlTSff+gqA9zQAy4DGDI65GKgYfvIs9QhqxMu63wOPmH4VWZsTRD/ZPP40AP/i5NJF/r4weoYUHlqWLBmiPQ7hTEaZzmkz60p60ZpDEz7UvBNGaKACs7WIS8IdM7gCMg1o1WuiHVh26Cs6qvFoum7STOVmybCBZR8wdsn16DNQZSDMkjBI15Z2OAB9a0dUUfPCR1j+U++eaoXUapaLdm2+2yxDdb256NJ0BOeOPeuFx1PRhLQvWk8Myh42LL1BIIBHt61i+JLfVZZoIdHu0sfObN7euuWEfZF/U9unWotMsdbidptb1T7beSsW8uHiKEdl9/wDPWtyMyTxeZtVlThstgVtezsRyt6mRPbW2n2lrdu01zFZPvaab5nxgjd+Gc1PLe2d1GqxAXMFzlXG08KR1Oe1aQ2FTE8YKycL3B9q5+xu3tb+60S7Ake0bEco4LREZTcO5A4yPTpUNWN1aQ/StHuNMkfytTlntgR5cM4DbF9M9T9TW8shT514b2qhH5kbbcbl7H2q1GJJDwOfSkmyZRXQ5W58BRaxrJu57lraNzmTyBhm/p+NXNP0zTLK2u/I0dIEjwEnuF83zxnHBfP3uelS6rrawymO3lyYzyy9M+nvWZous3Xibxv5d3LutbK1LLEvClyQAcd8DP51TvLQFaGrR1ehWMWi6LHbW0Sxjk4HQE8muZ8d+PD4bxpOmYl1iZQTIRlbYHocd2I6DoOD7V3m1GRT2HavnbSluNc8RT396xe6muCXz/fJ5/ADP6VpprfocuraS6nrnhewaCxikmYvI6hnZjksx6kmushHArLsE2QxgDooBrVhGW9axpqyOirK7NO3fcpXuOlSv/q2PtVe2+8/0FTscxN9K7obHmy+IrjrQ/wDrk+hpV602Q4mT6GrJLo6CijsKKQBRRRQAUUUUAFFFFAEUnUn86gIJbjvU8pGeelRZwMmgCC5YpEoHdwOKrS5E0X0P86sT52rt6lhVeYfPF9DQBKpySaWEYuY/dhSLw2PanRf8fUYP97imI0j1pKU0UhiUUuKMUAA61nXE6xAA8nPHpVi5uo41KlwoHDGud1PUw5WOIH53CqfesKslY3pU22GrTbrdnXDALuQZx+tUNKuhPEQJN207XVuGjb0I9/WtUW6yaZHyGK7lYA5xk5/rXPaj4dtXSO4k3pI0gAZWIz7/AKVj7KbldbHRGrFJxZsqq7JPYGoYpkBMUc8ZUnafnAVMdR/vY5x1qnp2sytDv1m0ksJslSXHyyL2bI+7kdjjmnQaBpEkkslqiiOchpkib5JiDkFgOCarS+prdPdk9hC11rsuoLL5kEEX2aLbny2YOWLqD3I2gn271j3EsN1qD6nbkM9xIV35+UxqP/rVuatfW3h7w3dXczpBGkZSAZ+85Hygf57Vxug3ED6dpNmzgeZzt/2Sc/yBrWKi2+ZGM5NaxZ08RndlVO67slTwKw/En/CTva7bXzbXAYsIxhZ1Ho3UfQ13lvBGGUxAAEDGOmBU4iRyygBhjkEZApxUOxhKpPufO9x4hvEYwNHjIyNwKsB9PWut+EZe5u9ZvZeSiRRqfqWJ/kK7/wAVeANG8XQPJdRm31MR4hvIzg8A7Qw6MM/jjoRXH/Cezks9H1dJwBMl+0L/AFRRn9TSkkolQm5PU9Gt/mYZrw/wvat/wmGpqw4t7iQY9GLEfyr261YBl9DXlmk2rW/xE8QqRhWvGYY9yT/WsJfAzopr30ei2gwi/StOE7UZyQABkk9qz4BgAe1acNstymyX/VjBZf73t9KIK9kKo7K5csx+5MhB/eYIz6dv8+9Sv/q2oJIXJ6k0H5o2ftjgV2JW0OBu+pCOtNf76H2NOFMkP72MdiDVCL/YUUdqKQBRRRQAUUUUAFFFFAEEvysT1qHluPWppPvMO1RdqAK90SLdQvUuBUMoy8X0NWbjP2dtq5bIxmoHGWj5/hNADx9/8KfD/wAfMf1qMcP7Yp0B/wBLi+v9KYjTJABJIAHesu71h41JsrY3O084YDP0z1qLWriTzRbq2EC5bB6msjcydD9MVy1ajTsjrpUk1zSL8fiVpGK7ArjqjLhh+BqWLWZLoSKmV2LliO1Y1zBFfx7LncHH3JkOHQ+xqbTI5NO0+SKaYXLu5Pmhdu4cAAj2H86xhOblq9DolTpqOi1LZOJpYzyFAYfjmsCGC5uvGInZ0Gn2KFigJ3GTBUDHp82fwrZNx/xN5IQPvwhlz3AOD+RI/Osyxfyv7caWQJPDNvI/vrgBfrWm5UfdTNXQ5DPHeoUICSBkb1yOcflUl62byCSQZhjHzHGeT7fSsrS9TaJWWNGkTA+aMZGeeM+vNUda8QFriC2tlL3St5nkjso67j9K3dSMY2juc0KMqlRt6I6oPbzZTzEYv2IxkfjWZeeHLW6bzkXa0TEwhfl2nOf5iqk15JG2+SyaeLGfMhOTn2Wr0Msu1ZYZnAYDAbsPoelZKono0U6TjrFmU2m28l6Li8jM5KGKYTfOYc9eD0/D2rQt9EXTtShniWNeGjDYAAyOAB+Yp7Aea8n3pJeXJ78Yp63o8gWk7AnI27jg8dDSi0tAqXepqWqbYyv3MHkVciQL3yf1qhZSCWASl9x3EZ7f54q4Hd0G0lAO/etkcrJjhnAB+uK5b+zodK1bUYrZFjjupRc7V6bmUA/qtdOhAGFHHp6VgX80c2rSrEwYQqEYhsgNk5HsRWdX4TSh8RPbttINcpBZRp421aQjmZ0k590H+Brp0bj8K53WLWdfF1jfW9xJCJ7cxMFGVLKcqSO/3sfSsJ7HbS3Z0cS9O1bFmP3X1NZFuTJGjsMFgCR6Vq28gUKgPzY6VvSWpzV3pYlMqz3PlLyqdT71O/ETfSmxxLGNqjAp0n+qbFdCOQgBxTJM+anpg04daR/vr9DTAvdhRR2FFIAooooAKKKKACiiigCCb7xHem4HA7dakkHz59qjPH5UAQ3bZhwOPmFUz/rI/wDdNWLtCbY/UVCRzF9CKAJAMtn2pbfm9i+p/kaB/rPwpbcf6bH+P8jTEGqaP9ubzoJzBOB1I3K31H+Fc/cRajZN/plk5XOBJCPMU+/HI/EV2RoyaxnSUtTeFaUNN0cRFcwTj93ICR1GatWzAOUk4Xk57YPB/LiumubK0u123NvHJzkbl71l3vhuC4iZbWVoCwI2tl0OR09R+BrH2Mou61N1iIvR6GLqVwIILTUMEy6fPiUDr5Z+Vj9MEN+FYfibTrm98UQ7bho7WaDMiR8EsDg89cHj8q6d9J1KIRJc26XEUqmG5MLbtowdr4bBPoQM9fasaCa4uDA97C9vJbRmBfMVlaQA4DnPqAtKSkkdEJQautTUiiFvZxw26ooC4VOwqrfEnT5ReWwjXbzcRMSY/wDaqXzYZIwgUzBjhgGAx+dUtQnklWaz0a3uLm8gAMkAjPlsp4wW+7+tJK+wr2d2UtIS/t9PiRbspglV84B45QDjII5GeuCa38kxqzDaT/d6VlWWhaotnGJrGQybQkkRO1cDptIxgY4xU62+oWkZgi0S6GOQqkMPwOafI09iXUjLW5ejZe/B/Snz28MsIWRcsOVb0qiZdahVSPC19KG6mOWHj8CwNTyzSrCGNpdIT1UwNlfrx/Knyu2qM1JX0ZRg1C68P3RknL3enu3zH+KHJ5bAHzACuwSSKaOMpKhR1Dxnd94EZ4rkJr2JDtlV0J/hdSD+RrE1CLTnYOD5bLkoQSCueuPSlGo47lSoKeq0Oz8ReLtI8N2xk1S8WCbaXiiCktNjtge/WsTw7qb65oq61Iio97IzlVAGACVHT2FeY+KLWz+xymNg8o5BLZPr/jXbfDK4E/gSBN2TBNIh9udw/nVTlzwuRGn7OfL5HYqfk5//AF1U1RSBaTqN3kzAt9GG3j8SKsIc065XzbKZT/cLD6jkfyrJ6xNou0izboQioOGI/KtWws0tIAAWdjyXfksfWqGmqJnRn4ULuNaoYueOFFdVJaXOOu/esSZpJD+6alHSmyn901amBAOuaa/+sX6GnCmv/rEHtTAv0UUUgCiiigAooooAKKKKAIpMl8e1Rk9u4qSX7xNQMRwaAI7wB7QrkrlhyBmqx+7F9TUt0SYtucDI/nUJ6R/U0ASg/OPpT7f/AI/Y/wAf5GmD/WdO1VtQv10ixk1JojMISB5YOCdxC9fxqkm3ZEyaim3sjcySeKMevNckPiDAeumTD6SCnj4gWf8AFp91+BX/ABrT2FTsYfW6P8x1QGKOtcuPH+m97K9H/AV/+Kp48e6Uetrej/tmv/xVL2NTsP6zR/mOkOQeKDhhhgCPQiudHjvSD/yyux/2zH+NOHjjRT1+0D6xUexqfyj+sUv5kbjW9ux3NbxMfUoKeMKNqgKPQCsIeNdD/wCesw/7YtTx4y0I/wDLy4+sTf4UvZT/AJR/WKX8y+82smjJ7VjjxboDf8v2PrG/+FPHinQT/wAxBfxRv8KXs59mP21P+ZGpyf4jj2oIJ74rNHifQj01GIfXI/pTx4i0Rv8AmJ2/4vijkn2Y/aU+6NA4P3gDj1FMeKKUEPEjA9ioNVBrmjN01S1/7+rTxrOkn7upWv8A3+X/ABpcsuw+eHczdT8EeG9Vt2hl0izQnPzpCFYH1yMGuUsvDcvgaK4tgm7Tp5d8UqEttOMYbPTgD2rvxqWnEfLqFsf+2y/409byyII+2QMD1/eKc1nOnzKxtTrKMr3ucjDdRNGGDjFTG4EiPHFukdlICoMnn2FdGbfR3YN5dmSOmAtSWtvZ2imOzWKNWOSEI5NYKhLudDxMOiKOl28oiZ5InjzgBWGDgd60lzjGQPpTyhPINO2H2rojHlVjmlJzldjB70kn+qNSbKZMuIWNMkrg802Q/vk9SKXv+FNk5mT6UwNCiiikAUUUUAFFFFABRRRQBFLgZ9TULDAzU0o+YmoXHr0oArTDeeWCgc5NQnpH9TU04B4dSUBGcVC4/wBXjoCaAHp94fSszxSf+Kaufdo//QxWmv3hWX4q/wCRcn/30/8AQhWtL416mNb+FL0ZxQ6UYoHSj6V6x8+L+FGPagZJAHLHgAdzT5YJ7cqtxbywlugkQrn86XkOwwdKXigUD60AGB0xRgelLz7j0z3o470DDAPapktVeGGQZ/eSmN+nyD5cH8dx/Kohz3pCpzgqQ542kc/lSYItJYQyGMebtLzCJgQMgFsBh6jg/THvTPscZimfdgxH7jDBYY6jOOckcehqEqASCOcYOeopePypWfcq8exZl0+KPzv3oJjKCLK/60tnA9jx3qK4tBbSmNtrgYw69GyAR+hFRjjoaUcChXXUHyvoN8pP7oo8mP8AuinEgdc+tOp3FYj8mM/wijyI/wC6KkpRSuOyI/s0X90UohVemR9DUnaigdhAHX7ssg+jmtXwy8p8Q24aaVl2v8rOSD8p7Vl1qeGP+Rih9kf+VZ1PgZrR/iR9TtT1xTX/ANYv0/rS01/9Yv0rzD2zQooopDCiiigAooooAKKKKAIJcmQ+gFRM2eO1SzMQ5Haq74AyaAIp/nQoWCjIyT0qHsD23GpXIxkruz0U96gU/KPqaAJR1rK8VH/inpfeRP51qLyx+lZXiwbfD7AnrKn4c1rS/iL1Ma/8KXocYOlKPSkHSl616p8+WNOgW61O2hcgR798memxfmb9AatQ3UOoNcpLHJ9lLSX1yztli2MKFxjAyQPfNZ6s6H927IT1KnBIpPbkA9fepcbu5pGfKrF97SH7JFPFaOz3keYIwzN5bbti5bp1BJzk/MAAOtWbix0xFmaKN2WNZ2B3k5RMKrY/66cfTJrI3yBQokcIrblXccK3qB2NKis3yCTaCMHc2FwOcfTPOKnkfcpTj/Kaf9nNN/oxjczRW8KoCxwk0hz09MZz24NKbHT1ineRZVVDM0bBufLQhFOO5MnAH+FUNkwJIu13Egk+dycdOfbtSeS2P+PiMjpjzOOuf58/WlyvuVzR/lJL2zVdVexhRkAdY9pOSDgbufTOefStaSRf7QfVYwGlexV4B/zzYqIwT7liMfRvasdUlSTzFukEnOZBL83PXmhY5FRkW5QI/wB9RJgN9fWhxv1CM0r6F6PSoY5Y0mjlcLcPHIzEgSpGpMpHfrwPp60zybY2qzXULRgW5upWjOCSz7UQdumPzqsRcO25rwMxGMmYk9MH9Bj6CkMcjDa1wjKABgycYHQfQUcr6sOZbJFuSxtIZ0hlaVdzIzMOREjDOGOMcZQZH+0fSopbWOK2uJGjdZoZfLKFs7OwOcfMu5XGfYe9MBuV2YvR+7XYn777i+g9B/hSFJGjWJrlGjTlUMnAP+c/nQk+4Nroi1aXK6dpsM0jS/vrkyCOPpKqDG1jnhSWIPB6UPY20eQBMZl8rfEpAHmSDiNeMjHP5AVVKSOFV7hHVBhFaTIUe3pSqsyM7pdKrSAh2EvLA9c+tLl63DmVrWLUlhBHGQJMrH5kjzs2AyB/LUDg4ycknn+VN+wwG7it1NwWuSGh4A2xl9vz++Ax9uOKgQz24WSG62GNdi+XJyF7qPamLNPHGkaTSIkZ3RgMcIfUelCUu43KPYufYY5nYxB1MiiSJM5Cq0mxE9Sx5P4d6rXKW0dw0dq8kiISC745IJ5GO2MUwSShVQSuAh3IAx+U+o/M/maaAAMDimk1uxOSeyFrV8LjPiGP/rk/8qyq1vC3/IwKf+mL0qnwMqj/ABI+p2Oct9Ka/wDrF+lKPvfWkf8A1q/Q15jPbNA0UGikMKKKKACiiigAooooArT5Mh9BUDAtxVqTG5h6VVc459aAI9uQWPUVXXOVHXOasgcMenFV0zlT2waAJIxtbPX2rI8X/wDIE68tKta69axPGUgTRULEAGZefzraj/ERhiNKMvQ5IdKKiFxFj7wo+0xY++K9U8C6JqKi+0Rf3hzSidPUmgZJ9aXqKYJM/dVj+Bpw3npFIf8AgJpDFxxSjrQElP8Ay7zH/tmacIrj/n1nP0iNK4WY0CipBb3Z/wCXO4P/AGyb/CnCzvj/AMuNz/36b/Ci6HyvsMGMUuBUgsb89NPuf+/Tf4U4afqJ6addf9+W/wAKV13KtLsQYHpS4HpVj+zdUP8AzDLs/wDbFqX+y9U/6Bd2f+2TUuZdx8kuxWwKAPSrI0vVf+gXdf8Afo07+ydWP/MMuf8Avg0uaPcfJLs/uKvHpS1bGjauf+YZcf8AfNOGhaz/ANA2X9P8aOaPcfJPsylS1eGga0T/AMg6T8WX/GnDw9rZ/wCYe3/fa/40uePcfs59mZ9a3hXnXvpA/wDSoh4d1z/oHn/v4v8AjWj4f0jUdP1Y3F7beVEYmUNvU8kjjAPtUVJx5Hqa0ac/aRbR0g+9SN/rU+lKOaD/AK1PT/69eceuXzRQaKQwooooAKKKKACiiigCnO2Zn7EcVASc1PcL+8P51AQc80AKvLH0qqPvD05xVlepJqvks4/GgCRTmgSwQzGa6ZVhVTksMgHikHBrO1yNGtUJKgeYM7yMH0xnvn05qlqyJy5Ytmz/AGppKgN58OCcAgdT6dOtQyapbgjZqUKfMSB5eSw54+o4/KuXT7zz7lI/5aNtLFO2cA8ZyM4GTgU1dXOmXMgkjhjDgGG4mkClwRzgngHdxjOelXyHG8S0rtHVnU4QxR9RKl1G3EB4IPJ5HemrqEbME/tUls7cfZ+SeenHuPyrnE8QT30n2G1jW5ldgJCTnyB3Jx0PYDqSR71MyLLLKpgdZBGfNDHDxqOSwOPXoMjsaHGw44jnV47fM2zqsEt0UTUJ0X7gBtTy2CDyR1yR+VKuoRK3zaq5bjAMQw3Tgccn5Tx/tH2rn/7TsdOZbfUIT9idAbaaQtiQnOVI67u/PXOamiuWmtVmms3sRISYomGWiX+EuB0Jx07A9aXKNVm3b/M3IdWtbeYwzXkssr42o0WGHXPGPz9Pxov/ABRpWl2El/fzNb2sf3pWQkdQvAGSeSOgrFQ/IqQuobGYzu6e+M8gn3/nXPeMooLjwxq9kWiOpsY2e2jyrMm5WLKuSSvuB1HPIpSVk2aRqybSOysPHPh7Vrd5tM1BbwR/eSMYkHqdjYY+vAqwl1A20m6u9jg4YsAuOe//AAIfkK+crbQ5PPhli+2WUwOYpgpG1h0ORyOe4rrNV8Za3/witzpusQWz3cxEKXcR2yXC4yxwBzxtBOR97v25vadjqST3PS9T8YaRYW97cSS6lJCnzGaBcpyAFEbfdOeowT3NYUvxj8NODOkGsHLfdQKB27buPu/qfWvMNKmv4jFY6TIJX8pt7lsQwRE5d33fKAT3YdABVtvB5+zzSQapY3yWyCaZbItjBOM5YAbR7Z+lR7SS+Jl8kWtEeteHPHmi+JJ/Ks1v0fcF2TbRj34J9P1rN8Q/FfS/CHiC70aXT766mg27pBKu07lD8Z/38fhXCfCtDHr11qjh447WPykUj78knCDH5n8DVz4gaJoV3qM2tHUZWlklEF3IrBvKlCgKNnXaQByDQq1puMmDglG6OjsvjnY399HaQ6FdbpM4LTKOgJ/pW+/j67DQxx6EHmnTMMRvFUzNjO1Pl5IUgnOOoxmvBrK1vtH8SQqIybmNHkgZULCX5GKlR3zXWzahJJplteazctZ3Uh+Xbu81ZAQd6p2K8Z9enGKK05prle5CPRl8fvJNFJc+H7qGBX2SOs4aSLJADNGOdpPfrgZxioNT8d28AY6ZodxqxL7C8UxAIOck8Z4OQciuUtTLqNxbSvDDBd6jmKZXA8udFCjdHGcElgQNvY5+la0uhPayWd88L/2oojjn0+2/eBHlyrSPj+HGcHoDXK8TUT1Y+VPobtrr3iS/hWdfCdukIBKs2pbsgnJxtU55FMl8Q6tZWzTXfhu2UxsPKEdwzAjrnoMcge9c3af8JfpWoS6bEraXb2Ls1vsi8y0MbHOGz2ABO7OR83c10Wh3t/4j1O7v7q6gTTo4CsVipG7rxKy9Vzg49v1ieJrrXmVg5Y9iTS/H97fahcWk2mRQmO3WeMiUncpJVs8djj86s6L4tuNd1yXS5rSOFY4WlDIxJOCB/WsfTk0i9ji12N5NojdbVuUVkbruU9enGaPCFxDN42uBCBzZuSf+BLV0MRUnVSYNaHcjrRjMqf570Dk05SPPTvXqEl00UGikAUUUUAFFFFABRRRQBVlIaZuelV2ILZB4qScjznPTnH1qEYyTn6UAKOHI7YGarA5cfjVgEbWI/wCBH8OlVk5f8KAJe1Y3ilQdPgfC+ZHOHjDdCcHI/LIrZPAGaq39kt/HEv2iS2eF96SRBSwOMfxAjv6VSdmZ1YuUGkc39reW7F7qWnrcllxHbWpA8k4G3k4z/ES3044p2GQIl1Ks7ldu2TJMXfCqBjBJ6vxnHPAA1P8AhHrPy2iM9yd53PIWG9j/AL2OOeeO9PGgQbZB9uvj5+PtBMg3T46bm259uCOMDpWjkjiWHqdTNUyZjisQNNlhYsJQisshOQPlB7A5Oe/rUgsxLGIZi0pVi7SyOxaUt13YwMZ6DkdOOK2vscIt2t1j2RMACqjB/PrTRp9uP4X/AO+jS5kV9XmY/wBsSOMTR3ETTmQqbWKTa4K/eJB6HAPzH1HY0RrPLcvEbgwxzzlmsV2kLJ0Hz9TjAJHQlTzjNbA0+0WR5VgAklRY3fPzFV4Az+FJJpljLbi2e2UwgBQgJAAHTp3Hr1pcyL9jMzZJZrRmF6I3MW0yR2oJYKejAHOScE4/L3wfHd5dQeB7q/tpPJw6IDj5wTIpAzng46j3PpXY22l2VnEIra2WNAd33iST7k8n8aSfSNMu9y3lhb3CP99JUDK3pkH6D8qTaasVGjJNNs+eP+Et1UshN8xEf3QQOOMVRutTed1l84+Zg5PQcnmvo4eGfDiHKeHdLU+1on+FSpoujRnKaJp6n/ZtUH9KzUIo6T58e4S208WT3LC3JD3Wz/lrJjIQY67Rxz3zViDXporCERzxQJbkIN3z5P8ADxg7iufTA4xzzX0ItrZoQVsLUY6fuF/w96mVzGQY0jUgYG1AMVDpJ7lqdtj598S+ObvX9WgnsFNlDFFgRxjYZZSPnkO3uT09AO2TXoOlx6N4s061to9GuDdW8MYunwEeN1ULv2tgSLgdQSenFeifarj+/TJGeUAOxOKHSiLmZw994XudFjtdWkH2ptJY3ESwLvfbtIKKPfII+lcvZx+JNdv59Znsr+1c7YooDG5ZgHByWIHPUdOn0r15VKEMpYEGnszscs7H8al0IvYG7nCaNoh1DTZINd026ubnyxMFmRo/LbPHly9pPYYrX1KxewuNM1bS01G91O1hEMh25a7ix92Y8DIPOeoPaujIyBlj69aAo7E/nWP1ON78zDmMR7bU/Fnh2ay12NtFaWYYSBwzPEMZDfXkVmHTdVttc1k2GltDZ6kiW63cci74ljjCKVQnlcZ9859q64w7jnqfelEWKpYSC0uw5mczrul31/bxRaXa7VVArLK6qePx9KXwn4bvtG1d726jjWJ7Yx/K4YhiwPbtxXTCMD1xUgyBjtVU8LCnrG4m7ijrkdafHzMlMGDUkX+uBrpAuUUUUgCiiigAooooAKKKKAKNwkjyuQmRn+lQj7rdAR2PWtCVkGSTz7daryKkgPmx5zxlTzQBT81fJ2fdLZwBUcQ+XJ4OOlTXUUCx70d9wX+AFmAHbb3NYKeLdIiiD3rXWnyZwY7u0kRvr0NAG2GBorEXxp4XY4XVlZvRIZG/ktSDxdob/wCrN9L/ALmnznP/AI7TA2KBisr/AISWzIzHpmsyf7unSj+YFB8Q8fJ4d1yT6Wyr/wChMKBGrkUZzWWutXrjKeE9YH++YF/9qUv9o6265j8LTqfSW7iX+RNAzT4NHesz7R4nYfLoFmntJqP+EZpR/wAJY3P2DSI/reSN/wC0xSCxoOWVdyqWOelNMkmcCAnHv14+lU/I8TuRufSo/wDdMjf4U8WPiJvvajp6D/ZtXP8AN6LhYtLM+0Zt23EZIPbr3/D9aU3D4J+yuAPzqodK1hv9Zrqrn/nlaKP5k0n9hXzfe8RXv/AYoR/7JRcC8jtJkPE0eMY3d6cFOKoDw8+f3ut6lIPTei/yUU4+GrGRcTT38o/2r2Uf+gsKALZKjksKQzQr96eNfqcVS/4RLRP4red/9+7mb+bU4eEvDo+9pFtIf+mi7/8A0LNFwJX1PTYv9bfwLj1cVWfxHoEf3tYtB9ZRVtPD2hw/6vRrBPpbJ/hVqOxsof8AVWcCf7saj+lAGMfFXh88LqkD/wC4d38qcPEmmMf3ZupP+udpK38lrdAUdFA+lOyaAMZdWRuUtNQYds2kg/mKkF/O33NLvT9UVf5sK1fmNGD60AZyz3z/APMNkT/rpKg/kTUgN/8A8+sI+s5/+Jq7tNG2gCosV6333gT2UFsfjx/KrEETLNvLk1Jtpyj5vWgCxRRRQAUUUUAFFFFABRRRQAxo9xPvUJg6j9Ks0YoApNBx1LGhC6HAzk9aubRSFRQBX86Sje3oKm2L6UmxaAIdz5o+f1qbaKNooAh+ajDVPgUu0UAV9hpdhqYgCjAoAh2HvR5eKnCil2igCDy6NlT7RRtFAEGyk2VYwKAAaAIPLNHl1PtHpRtHpQBD5dGyp8CkxQBDspdlS4FKQMUAQ7KNhFT7RSYFAEOylCA9KlwKABmgBmygLyKkwKMUABooooAKKKKAP//Z</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_garden_sr_pg1_2?ie=UTF8&amp;adId=A02467633V7BWGZXSIAD6&amp;url=https%3A%2F%2Fwww.amazon.com%2FLINENSPA-Premium-Smooth-Mattress-Protector%2Fdp%2FB00MW50FKG%2Fref%3Dsr_1_2_sspa%3Fs%3Dbedbath%26ie%3DUTF8%26qid%3D1522624327%26sr%3D1-2-spons%26keywords%3Dmattress%2Bprotector%26psc%3D1&amp;qualifier=1522624327&amp;id=3898230458598911&amp;widgetName=sp_atf</t>
+  </si>
+  <si>
+    <t>[Sponsored]Tastelife Waterproof Mattress Pad Protector Cover (Fitted 8" - 21" Deep Pocket) (Full, White)</t>
+  </si>
+  <si>
+    <t>4.4 out of 5 stars</t>
+  </si>
+  <si>
+    <t>649 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin:$19.99/Twin XL:$14.99/Full:$19.99/Queen:$19.99/King:$23.99/California King:$29.99</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71qxSzxXtiL._SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_garden_sr_pg1_3?ie=UTF8&amp;adId=A04114602J3X5FPTHPUDU&amp;url=https%3A%2F%2Fwww.amazon.com%2FTastelife-Waterproof-Mattress-Protector-Fitted%2Fdp%2FB0716R1SZD%2Fref%3Dsr_1_3_sspa%3Fs%3Dbedbath%26ie%3DUTF8%26qid%3D1522624327%26sr%3D1-3-spons%26keywords%3Dmattress%2Bprotector%26psc%3D1&amp;qualifier=1522624327&amp;id=3898230458598911&amp;widgetName=sp_atf</t>
+  </si>
+  <si>
+    <t>Queen Size SafeRest Premium Hypoallergenic Waterproof Mattress Protector - Vinyl Free</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/SafeRest-Hypoallergenic-Waterproof-Mattress-Protector/dp/B003PWNH4Q/ref=sr_1_4?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-4&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>LINENSPA Zippered Encasement Waterproof, Dust Mite Proof, Bed Bug Proof, Hypoallergenic Breathable Mattress Protector - Queen Size</t>
+  </si>
+  <si>
+    <t>4.3 out of 5 stars</t>
+  </si>
+  <si>
+    <t>3,242 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin:$21.99/Twin XL:$24.99/Full:$24.99/Full XL:$24.99/Standard Pillow Protector:$13.99/Queen:$24.99/Queen Pillow Protector:$13.99/King:$31.99/King Pillow Protector:$14.99/California King:$32.99</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71wVDfmlzJL._SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Encasement-Waterproof-Hypoallergenic-Breathable-Protector/dp/B00Z06F2OI/ref=sr_1_5?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-5&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>LUCID Premium Hypoallergenic 100% Waterproof Mattress Protector - 15 Year Warranty - Vinyl Free - Queen</t>
+  </si>
+  <si>
+    <t>4,346 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin:$19.99/Twin XL:$17.99/Full:$21.99/Standard Pillow Protector Set (2):$14.99/Queen:$19.99/Queen Pillow Protector Set (2):$17.99/King:$29.99/King Pillow Protector Set (2):$19.99/California King:$41.99</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/61Vz4obG4mL._SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Premium-Hypoallergenic-Waterproof-Mattress-Protector/dp/B00A2G9VFM/ref=sr_1_6?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-6&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>Quilted Fitted Mattress Pad (Queen) - Mattress Cover Stretches up to 16 Inches Deep - Mattress Topper by Utopia Bedding</t>
+  </si>
+  <si>
+    <t>4.6 out of 5 stars</t>
+  </si>
+  <si>
+    <t>5,154 customer reviews</t>
+  </si>
+  <si>
+    <t>TwinXL:$18.99/California King:$24.99/Full:$20.99/King:$23.99/Queen:$19.99/Twin:$19.99</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/61HHRDK8ZwL._SX450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Quilted-Fitted-Mattress-Pad-Queen/dp/B00NESCOY0/ref=sr_1_7?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-7&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>LINENSPA Premium Smooth Fabric Mattress Protector - 100% Waterproof - Hypoallergenic - 10 Year Warranty - Vinyl Free - Full</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71gpwo%2BfcsL._SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/LINENSPA-Premium-Smooth-Mattress-Protector/dp/B00MW50754/ref=sr_1_8?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-8&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>Zen Bamboo Mattress Protector - Best Lab Tested Premium Waterproof, Hypoallergenic, Cool and Breathable Bamboo Derived From Rayon Mattress Protector and Cover - Full</t>
+  </si>
+  <si>
+    <t>4.8 out of 5 stars</t>
+  </si>
+  <si>
+    <t>868 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin:$16.99/Twin XL:$17.99/Full:$21.49/Queen:$20.99/King:$23.99/California King:$24.99</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71dQlD-UmsL._SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Zen-Bamboo-Mattress-Protector-Hypoallergenic/dp/B07B4L11BH/ref=sr_1_9?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-9&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>KISSBUTY Queen Size Mattress Protector Breathable Waterproof &amp; Hypoallergenic Cover-15 Year Warranty Vinyl Free</t>
+  </si>
+  <si>
+    <t>4.9 out of 5 stars</t>
+  </si>
+  <si>
+    <t>86 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin XL (39"x80"+14"):$19.90/Full (54"x75"+14"):$19.90/Queen (60"x80"+18"):$21.89/Cal King (72"x84"+18"):$28.90/King (76"x80"+18"):$26.59</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71UDfRtQNkL._SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/KISSBUTY-Protector-Breathable-Waterproof-Hypoallergenic/dp/B0785QMQD6/ref=sr_1_10?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-10&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>HOMFY Queen Premium Hypoallergenic Waterproof Mattress Protector, Deep Pocket Fitted Sheet (18”), Anti-Dust Mite and Soft Breathable - White</t>
+  </si>
+  <si>
+    <t>151 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin:$21.99/Full:$23.59/Queen:$25.49/King:$28.59</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71VYYOb6r-L._SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/HOMFY-Hypoallergenic-Waterproof-Protector-Breathable/dp/B075QG6Q8W/ref=sr_1_11?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-11&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>Queen Waterproof Mattress Pad Protector Cover - Fitted 8" - 21" Deep Pocket - Hypoallergenic Vinyl Free</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71zIcnXr6DL._SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Queen-Waterproof-Mattress-Protector-Cover/dp/B0722WRYVB/ref=sr_1_12?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-12&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>[Sponsored]One's Own Mattress Protector King Size - All Natural Organic Eucalyptus Fiber Top with Vinyl Free Biodegradable Waterproof Membrane - Hypoallergenic, Breathable, Thin, Smooth, Quiet Fitted Cover, by</t>
+  </si>
+  <si>
+    <t>118 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin:$64.99/Full:$69.99/Queen:$89.99/King:$89.99</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/91dD4UUdmrL._SX466_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/slredirect/picassoRedirect.html/ref=pa_sp_mtf_garden_sr_pg1_1?ie=UTF8&amp;adId=A0180995PZ9JHOP17BOH&amp;url=https%3A%2F%2Fwww.amazon.com%2FOnes-Own-Mattress-Protector-King%2Fdp%2FB01MG4YU4A%2Fref%3Dsr_1_13_sspa%3Fs%3Dbedbath%26ie%3DUTF8%26qid%3D1522624327%26sr%3D1-13-spons%26keywords%3Dmattress%2Bprotector%26psc%3D1&amp;qualifier=1522624327&amp;id=3898230458598911&amp;widgetName=sp_mtf</t>
+  </si>
+  <si>
+    <t>[Sponsored]Queen Size Mattress Protector LUXURY Turkish Cotton 100% Waterproof Hypoallergenic Terry Cover - Rapid Cool Tech - Vinyl Free - 10 Year Warranty by Run2Bed</t>
+  </si>
+  <si>
+    <t>73 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin:$21.90/Full:$24.90/Queen:$23.90/King:$29.99/California King:$31.90</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/91--zFzHUZL._SX466_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/slredirect/picassoRedirect.html/ref=pa_sp_mtf_garden_sr_pg1_2?ie=UTF8&amp;adId=A01525173MBA9NSQOTMHQ&amp;url=https%3A%2F%2Fwww.amazon.com%2FMattress-Protector-Turkish-Waterproof-Hypoallergenic%2Fdp%2FB06XBCFN3B%2Fref%3Dsr_1_14_sspa%3Fs%3Dbedbath%26ie%3DUTF8%26qid%3D1522624327%26sr%3D1-14-spons%26keywords%3Dmattress%2Bprotector%26psc%3D1&amp;qualifier=1522624327&amp;id=3898230458598911&amp;widgetName=sp_mtf</t>
+  </si>
+  <si>
+    <t>[Sponsored]Lulltra Bamboo derived Viscose Rayon Mattress Pad Protector Cover by Coop Home Goods - Cooling Waterproof Hypoallergenic Topper - California King - White-15 year warranty</t>
+  </si>
+  <si>
+    <t>2,045 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin:$35.99/Full:$39.99/Queen:$44.99/King:$49.99/California King:$49.99</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71PgbVC1DpL._SX466_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/slredirect/picassoRedirect.html/ref=pa_sp_mtf_garden_sr_pg1_3?ie=UTF8&amp;adId=A07061243VDLTF3MFESFQ&amp;url=https%3A%2F%2Fwww.amazon.com%2FMattress-Protector-Coop-Home-Goods%2Fdp%2FB00UKHSPJQ%2Fref%3Dsr_1_15_sspa%3Fs%3Dbedbath%26ie%3DUTF8%26qid%3D1522624327%26sr%3D1-15-spons%26keywords%3Dmattress%2Bprotector%26psc%3D1&amp;qualifier=1522624327&amp;id=3898230458598911&amp;widgetName=sp_mtf</t>
+  </si>
+  <si>
+    <t>Waterproof Bamboo Mattress Protector - Hypoallergenic fitted Mattress Cover - Breathable Cool Flow Technology - Full - by Utopia Bedding</t>
+  </si>
+  <si>
+    <t>1,909 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin:$16.99/Full:$19.99/Queen:$20.99/King:$21.99/TWINXL:$16.99/KINGCAL:$22.99</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71Iw5Np8lqL._SX466_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Waterproof-Bamboo-Mattress-Protector-Hypoallergenic/dp/B01E02DU0K/ref=sr_1_16?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-16&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>Maevis Bed Waterproof Mattress Protector Cover Pad Fitted 18 Inches Deep Pocket Premium Washable Vinyl Free - Queen</t>
+  </si>
+  <si>
+    <t>4.7 out of 5 stars</t>
+  </si>
+  <si>
+    <t>122 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin XL:$19.69/Full:$24.69/Queen:$19.90/King:$23.99/California King:$29.69</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71pGgRlIiTL._SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Maevis-Waterproof-Mattress-Protector-Washable/dp/B073SSD95M/ref=sr_1_17?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-17&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>Premium Full Mattress Protector, 100% Waterproof Hypoallergenic Mattress Cover with Cotton Terry Surface, Breathable, Vinyl Free, 10 Year Warranty Offered by Lighting Mall</t>
+  </si>
+  <si>
+    <t>99 customer reviews</t>
+  </si>
+  <si>
+    <t>Full:$20.99/King:$29.99/Queen:$24.99/Twin:$19.99</t>
+  </si>
+  <si>
+    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDAAoHBwgHBgoICAgLCgoLDhgQDg0NDh0VFhEYIx8lJCIfIiEmKzcvJik0KSEiMEExNDk7Pj4+JS5ESUM8SDc9Pjv/2wBDAQoLCw4NDhwQEBw7KCIoOzs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozs7Ozv/wAARCAEsASwDASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD2aiiigAooooAKKKazqn3mAoAdRURlOMqhx6t8oqNp8nHmZ9o1z+tAFgkAZPFM86P+9n6DNVXlVD84VSBnMjbj+VMN3z9+RucfKAOf8/yoAvCaM/xgfXinBlPQg/jVD7Yo/wCWzc/3lBpRcRt/HF/wJMfzoAv0VTWVT93yj/uyYp+9v7r/AINmgCzRVfzj6uPqoNKJ/wDbH4oRQBPRUInB7xn/AIFinCTPQZ+hBoAkopu//Zb8qN69zj6jFADqKbuU9GH50tAC0UUUAFFFFABRRRQAUUUUAFFFFABRRRQAUUUUAFFFFABRRRQAUUUUAV7yTyYvNJPlpy4XqRWXFrtvNJ5dvDccfeaOAsE9AW9f8mtK/jEkSjZ5hDAhDjDfnVC4tJlkW6lld2Vl8u3DlVAGew4PXvxwKAJPOaXBRPNB6MxLceuBSfvm+V5tv+yvX9P604XELRIziWV2XOwDAHtSrcTsdkcaQD2GTQAJZk5xGcE5O47R+VOKxL8v2qJWUZwADgVG8Tu37yRpT2Bbj8qNi4fCgKY2AGPagCc2r8fPHjtlMVGbQjgJCe/Dke9aI6CigDNNpICSYWye6sP8+1R/Zdm0iKRdvQ7M4rV2r/dH5UbR24oAy8lcZlkBH97IFIJZFGFuV69Cc8fjWrt9zSGMEc4P1AoAzt9wT1Vh6fL+NLvnA+aFD/uqf8auG0hbrFGf+A002UPZNv0YigCr5zqM+SePRsf54pReYJGJOP7pz/OrH2JR92SVfo1IbSTHFwx9mUGgCL7aO7t7ZUGnC7jJIDKSP9g/0o+yzDo0R+qYppt5sbTFCwHQBiKAJPtKgEllGP8AbIp63AY4U5PorA1W+zyDn7If+AuKY0SkYeGcDGMEZHTHagC/5pHUOPqtHnDuw/EEVmlYRgb2THqhFKCv8F30PA3EDFAGkJl/vL+dODg9B+RFZ4MpPEqsPYj+uaT/AEkYyiN6kjP8qANLd7H8qNy+v51nebMB/qDnvjIpReMOqvkdQrZNAGjuX+8Pzpazxedsvj3ApReRjPzqD7of6UAX6Kpi7XGdygeuSP50q3oMnlqu49ThgRigC3RSUtABRRRQAUUUUAFFFFAEM6BwBkqecMOo4rPSJkbzY/3kijgyMeT9e1aUvb8f5GqQKoVUHgHI96AI4VeJH8wRqXYssacqg9Ae/r+NPAwc5P0pFG5z8xx2Pc04DEZA65oAduHy9qZIMFuOdjfypTkY5/GmnlCf9hv5UAaQ6ClpB0FLQAUUUUAFJS1WuEM8iwZIjxukwcEjsP8APp70CbsTLLG5IV1Yr1AOcU7NZ9yxg1KzVFWKBY5HkcADgbQF/Etn/gNMs9UE9vdX8mRapKY4VC5Ztp2njrkvkY9hVcrtcjnV7M06KybKW/1ONrsXC20RJEKIiuDjuSeo+mM9vU6VtI8sIMihZBkOB0yODj2ocbDjLmJaKKKksTAo4opk88VvGZJpFjQfxMcCgB9NMaN95FP1AqIXsJxkugPQyRso/MipBNEZjEJE8wfw55/KiwroY1nbN1gj/BcU02EHZWX6OasUtAyr9hX+GWZfo2f50hs5f4blv+BKDVuigCibS4HSSJvrHimm2uO8MLfRiP6VoUUAZhgkGd1mee6uDRCCt1/qZIxtOdw+Xp2rTqOX7v5/yNAD1+6PpS0i8KPpS0AFFFFABRRRQAUUUUARy9B+P8jVNVC4PXFXZOg/H+RqipCxKAOOoB60AIgOCBx/hS7sEKScHgmhUKsQ2Sc9fah0+YcjA5PvQArdMDqOtMzlD/uN/I04tufHQdqQjCEdgrAflQBojoKWkHQUtABRRRQAlQyxyeYJIWUNjBVhwRU1ZlnbSaYLlI4p7h55mm3NKCuW7cn5Rx0A+lNEyZFrF2LGyYSt5jhHuJDj7saDLYH4hfX5qyZlubbw/YafGzJdzlYEYdRO4LSyf8ABc59fcVoXumTTQs1yfOa5kRrpowWCxocrEi9SMnrjnLE44FMu7a9mmuL+1iK3FtbPFYRSL91jy0hz/ESAB7Zz94gbwaSSOWabbf8AX9fqasVzp9oI7KKWKMRlYEjB4BA4Qe+BnHXFUD4jhR5FS2Yg3ws4Tux5r/8ALRvYL82T/smsyTT7mwKmxgaRNOsibMyKcyXDkh5Xz3AHfk7z61NaWqaXdNLcE/ZNGssQuRlpGYbpZfqcAfUt60ckbX3/AK/4b8SvaTvbb+v+H/DudOGXoCCajmuIoPLEjYMrhEABJLH6fQ/TFcomn3zRWU8jPb3mqSsbibcQbaE5k8tfRiFVSeDx7DE63l5pk0Vrb20VxNc3LLaxGTZlAp3yEY+RRgAdTj3ap9l2ZXtn1R0sU8U7SLG4YxPsfHZsA4/UViJJcXmqidVUylnW3EgytvEp2tJju7HOP9n6HN/R72K7sJJ4iTEk0qiTs+1yCw9QcdaisZi9mt8kBto3jJzc/IUTJOWXtjJ7/iKlLluU3zWHz3LtcJpgbfLMWLNgZWIAbmI9ckL+OexqHRz9p0UCNd0cNw6W7DuiSEKc9+B17/jVbQrYaqt5qt3ExivSEtlfIbyFzgnpjeSzY9CKZBrtwDi1tofshna0so14MzAgZGOFRdrknByMY6c3y7xXQz59VKXU6SiuZvtZjuXtGW7aK0tg17eSqrLujQlUXGc4dgSB3C++KtnxNHHtF1bNbsw3YZvujvnjrkqvGcs2ATgkR7KVjX20Lm5RWFba0xv7qWeTFu8xgtIuBkR582QnsuSQSeBtHrzfuNWtbae3gcs0tzjylRdxbJA7emck+gJ7UnCSdhqpFq9y9RRRUGgUyX7v5/yNPpkv3fz/AJGgBw6ClpF+6PpS0AFFFFABRRRQAUUUUAMk/h+p/kaztzKRjkt0zWjJ/D9f6Gs0LhgR9cZ5FAEkhIiBB+YnFORScBvvelMbG/JzgA04DcgNACMMnb1Oe1DrtyP9lv5GlXC9/wAT6U08J3JKNyfoaANEdBS0g6CloAKKKKAEqKUpvAlI29gehP8AWpqSgTRVu7MSL5kMzW0y8rKvT/gQ6MPr+GDzUNpfC5byLoCG5jOHjDcMezKe6nnH5HkVfdd64yR7jtUNxZQ3SBZ0D4GAe9UmtmS007xHhlQpG7je2cDuazzqzLfPbGANsbblTknnnj2DIf8AgVXLaxt7QlokwxGCT6VOUUnJUZHfFGiBqTXYzRqTzQJIbZWSTGFJJOckcgKfSn3DWyXUiy2cZaYLGZOMuuCcHvxjpVtrWB4/LaFCnpiiW2jmILqcgg5UlT+Y+pouhcsijDq1hDEkUcXlQonAULtRRx0B6D8hRcR2THybiCeSPAYRNlkOcnG3PPQ8HjirjWUDAjZjPXB9sfyNLParMd29434w6HkYz0z9TTur6C5ZW1IZLy1uIXiWdv3g2ZiBLLkA5HHowOagWy02CG0ghlWL+z0HlEMCUXaRznrkZ5qVdIt0ffGWU7s44IHLHgHp979BSNpW5/M88+YCCDt44GBkfkfwp3XRiak90RPo1ncedKm0rcNFJjGVzHgqP93jp7mnmwV7+W6EgM00IhZivQKSQV/Fv0FTiO4trVAjec6klgeNwP1zVd7i9ul8m0t2tj0MsoHyepA7nHTtn6YInJ9Qait0U4dCs4PLtJHjkQWItXjLchMnccf7Xc+3erdnprjU7vULh1LS7Y4PLP3YVGcHjqWLE49h2q1Y2sFpAUhXqcu5O5pG7sT3J9aljydxAKgnoRjnvSc33HGnFW0JaKKKg1CmS/d/P+Rp9Ry/dH4/yNAD1+6PpS0i/dH0paACiiigAooooAKKKKAGSfw/X+hqipXPzcHpk1ek/h+v9DWfyrDBxgcehNAAVO4npg8j1qRGJ4znjk01RnBPAPUelKOSSDnB6e9AClQDxzntTAQdyjJ2q3X6U4t1xximBQNx7lG59sUAC9OtOyR/EfzpF+6KXvSGO3v/AM9G/OnCSQfxmmUtAD/Nkx9+nedIByw/Ko1GRntS4LdOtMQv2mQH+E/hR9qkHULWDqPirTNNk8suJX7ndtX8+9Zn/CwbUP8AvLIGHIHmRShiPfFR7SO1y+SW9jsDfOP+WY/Ol+3HH+q/8e/+tVSCe2vrdLmyuEuIH4DxnIz6H0NOKntVElr7eO8R/OlF8h/gaqefWkPtQBf+2xdw35UovIc4yc/Ss8nI96WPls0AaP2iL+9+lL50f98VSz2paBF3zY/+ei/nSh0PRh+dZzc9qQH2oA0gVA4IpetZw2kdPrUTwg/cJU9uaLjsa9FYm91YguwI/wBqniWXHEr5/wB6lzBY2Kjl+6Px/kaxlurjzyPPfGOmat2880kwR5Ny7ScYFClcLGiv3R9KWkHQUtUIKKKKACiiigAooooAZJ/D9f6GqKgqo4zjpV6T+H6/0NUo/nU78Bh1x09qAGj5lJHAXke5pysuQB26+1BADDPIpE+Uc9Sc+9ACbed3A56nqKC24sPRG/kaXg8ccjOKbnLEeiNzn2oAVPu0vamxZK08UhhS0u2k6nFMQ/ooFYXiHVfJb7DE6oAu+4kJwFHZf6mtqSZIY5J5DiKFC7H2AzXmTXwu9+o6i5SJ28zyu8rE/Kv54P5VlVlZWRtShzO7MTxFN5cu9/lLcqGJDMPp2rmLm/LSLujVQP4wf8ea6DXrdNhuXy9xOScZzj2Ht71ykwZD85Zffp/+uueCR1T2O5+G+vf2b4mNizkWmpHaydlk/hb654/H2r14jBNfNsUksUlvPAzK6H5WxjB6j+VfQ2l36arpdrfoQRPCjnHqRz+tdEH0OWoupZIyOab7ZqXb+7aR2VI0GWdjgAepNc1/wsHwmbh4DqDgJx53lHy25xwR25znpirbS3Mkm9jezTo+FzUaPFPGs1vNHPE3AkiYMp/EVOq5HtTAFJJzTwMnqABySTwBTcdf0rmfiBrUmleGTa25IudRJhUjqqY+cj8CB+NDdlcaV3YzNf8AibBbyTWuhQrcGJtpu3+4T3wO496xLL4ra3FdOl5p9vdp97C/IcdwD6/WuWhs2+yoduEJwcfzrSOhvLZgINu0blGOvv8AQ4/CuZ1Hc6lRVtj1rQNesPEmmDUNOc4ztlhf78L/AN1h/I9DWkQduRyRXl/w4M2j+JzBISLfUYjGfTeuSpPv1H416iDtYg9jW8Jcyuc848rsUpZI3USK3zDgj1qsboryHHy9QFJA/Hp+tSX4zdCOJcliBgHGc/5xVkw2FtFKsvmmSLCsykjBxn5R0wASfz615NetVqVXGk0lHq+5tCMYxTkr3KkEgkdiMA46Ves/+Pgf7hrJlU2OobNwKnkEDAIPcD6fqDWpZH/Sf+AH+VdeErSqR97daMirBR22ZsDoKWkHQUtdxgFFFFABRRRQAUUUUAMk/h+v9DVJWOw5H3RV2T+H6/0NUF5AyMheTk8UALH82WY5wSOKapBkkJ9hgnpTowXAGcKo60MuVDR4U5GB6AUAAGX+UY7Z9+1K6hd2ByVb8sGlzhcg4zk/SmcYJUYGxvx+WgBRwgFSAcU0IGAJen496AA9KYevvSk5OAaTnNAGR4rvk0/w7MhTzJr0/Z4Y84DM3qT0GM815F5eorqrjWcrcRsV8kHiP24716n4xMcNlZ30qiRbO43+Wf4yVYAf99baxvAsMuoXN/4k1FE86dvKiO3jjq38h+Fc1TWdjspJKncw4PDuqasRMka28IGPOuFO0D/ZHVv5VXuvBMGXdLx2mbkzOgJP0B4H4V3esa0LAZvLeUwE7TNDiUL7sB8w/Ksh5En2tBIskT/MHU8YrNqxrHVHB61oEen20c/nPtVvmJ5x716J8ObxR4Olnu3EcFjv8xj2VdxJ+lcv4oTPhy93DgRlgfpUFvenTfg3KM4N/dLFyeoxuOPy/WrpvdkVoppIoeJPFVz4m1OW5leWKwUbba1ViBs9WA6kk/pisuyHmuI/KDFSVHoBzge3cflWfa3P2y58sA7AcYFdDZ2ZhlmUY3EAj65//VWcpPqOKXQm8P6xd+E9T32zN5MuC0RPySgdj7+jdvpXs1ndw6jYwXtvnyZ4w6g9RnsfpXhF/cxfaG7hvmAHY9eP1/SvUvhzf/a/BwjJybW4eLPqPvD+da0pO9jGtFWujqc9SfTFcr4nso9S1y3t3jMpityRg8Jk9a6cMHXCn5R1PvWTqiCDxDa3ajie1eJvqjAj9Gb8q0qK8TOk/fMH/hG7e0VAfn28kdv8/wCFVZ0+zyIAPu9h2HpXRXLNIm/ouOTXP6ze2VjsM7ZaVsIo7n+gHrXK0jvi+5Tuw1oba8tv9ZBcLKvuQQcfp+tegaTqcWu6eL+KJ7c7ykkT9UYf/WIP41xFvJFfWDMuDtKswVgwGD2I9s10Xghbu38OyLqM4kuDcsRIeNy4AH6CtaLfNYwrwXLzdS+4KazAzH5RJyfXOAKuXtrJI11hkBdwUBbr8hXn065qrqUW8LKhVifcdR/9b/GhfEKRW+2eNJJVwMswU+mWB5/LNea+SlUnCq7Ju6+6wJSlFOBW1mMrqdtbhiVS3CnnuM/5/Gr9gf8ASsHrsbNZdgkl/qzXMoO5zufIxwPbtngY69OvNbKoV1ZXUYWSJs/WuvBq7nUS0bIru3LHsjVHQUtIOgpa9E5QooooAKKKKACiiigBkn8P1/pVEk7NijnsPWr0n8P1/pVEBsjnk/KKABMKoRScLwxHel5JZScDr/hSL8nDde3oKVhtG8tx3HdqAGyYzgnbnqfb/I/WnMcj0BVsD/gNNP70lgDjoc0rMC7KDnCt/I0APUcDH5UZLHaBg01sqvHNPTKjHc9TQMesarwOT3NZ15q8MGUtwJZOm4/dH+NTXjsR9nQkAjLkdT6CuV1Gby5yg4xWNWpbRG9Klzasva6ra/4ej2J+/t59zRoM5x1x+DAineGrhL3wvY3EUDW0ckZCRsBkAEgEgeuM1H4buVdrtu0e1z+R/wABU2kMun+FbQyfKIYcN7YrO6lZmyXLeKOM8S6JNc6vHJYMbe+jZm8zzG2vnHOM9sdOnXjmtTxOw8O6Ja3Nvb+ZM4+eJABuPf6VJZTf23qcOoxMEsSxAkPOSOoPoc1J4ymEt3BGUBWJBuHbk1L2uafaSR51c3BvtAvxcQXtrNcFDmSYyRHLDIGQAD7VV1/XIbzwTpujFCl7aXO5So+SSPZtz7EED866LxXGi6La2iLs864BK+wB/wDrVyes2wjS3lUACNwv4GiMrSCcLxLPhTS9yvcMuXU8D1rUurtmkjCLhwdpxwe4/nz+Fa3ga2EyPuQlQueB1461M2k2upSG/wBPdJhbSZmMbhhx7j8ayd27lqKSscdZ6dJe3bS85SQgqP7p5Br0v4Vyedo2p2icGK+3/QMuP/Za5u1ubf8AtMtaaddGENg3AUCLOenJye9dB8O0hsPE+uQLMqR4DMrHAyxBH88VrTupq5lWScHY70RKoAHAHQVW1WD7RpxdAN9s4lX3AyGH12k/jVhrmDLYkB29cd/pWe5ee8Jeb90FykXQKfU+v411tX0OFaO5xuueJ7iwuYoYtPee2LYPljLA88nsMgHGeuKqeJ9E8zWrNrgJPaTRYCSfdJPr7iuqms4VuHimXYmRJImP9Zj7oJ9Biqmvm0udGjuLhy0XJBQ4bHUH/PrXI1Y9GMr28zPtLX7DN5alTkAvtXaOfarltqBtHezhcp5SCVkYZXaxI3D2yDn0yPWuasdSnS8itLiQPLLGWX+8q9t315x3rWuZAmr2Mv8Az0Z7R/dXXcP/AB5B+dKDtIKsU4nWQXEEtssjQgFh84BPXNC2qysrB9iZ6MCT+GCKydLuxFptuPKHmRHyW3H72DithLljMwRUB9uua2lThU+JXOLmlDY0IbaKzjCQ52Nzk9T9anjOW/A/yqJH8+J8HOPu063bL/8AAT/KtUklZGTberNAdBS0g6ClqhBRRRQAUUUUAFFFFADH/h+v9KprnYO5q4/8P1qipEgwp4AwaADcCpxySevrTQpYlm6Acc/ypQchdgyeQe1KpLbgT/u+9ACFvkVxgLnoPSlf7w4x8jcenFIoOeuVHb86Ccu3QfIx/T/69ACREySY7KMmrATceCQaitU2wZ/vHNTZyQBTGUJWInmz1z/SuQ1wHezDqK667wL2UeoB/SuX1oAbm9q4ah3UegzwTKZZNThPUwZ5/Ef1raKrJYrb5+WRQBXPeBJCniO4TPDwg/kw/wAav2l/GXaHcMQSNGQTyCDjH5iknaC+Zcl+8l8iC/trHw/FJKtvKtpdEC7+zcPDIBgSAd8jGR/sj8eWa4vNTvQttem7s1wv2maIoc/3VGe3c4+ldjrF7A0YVnCPj756GsPw6TqniG4gj5t7WJdz46uzcD8AD+dXfmfKPm5YuTMTUXfVdTGNxgtFMSM3V2/ib+n4VkeILbOnSqOoGa7BrIJqVxCP4Hkcn/gRA/rWJq8IMcgK5ABrF6SNlZqxq+BrddQ8O/Z7mDg/LJFJnDjqM+1dNo9jZWNvdwW0UVujhlkSJQqjjpgfWuS+H9/d3WoXUt3IFFxAoihC7VQqe35nPeujjuLi0spbV9NOxmLtfs2VZ84YEAEr2x7Vtaxg3fYyLDywkloyIHGTG47/AI+tXNH2tfahGsIZ4iocEf6wbQTg+v8AhWWpu7rUmeQpb2MbZUKuDIepbJ5Cgcfic1raM4urCPU4lKpcjzAPbJAz+FOmveFVfu2NSORLUsbd2EEgztkPMbf4VqafvNv5rKuX+YKBniufvR5dtIVxyDiupgiCWkS8DCAD8q6bnE1Yo6tH9sspPLYpKilcY7H0/wAK56GEXllHHqFoIbSCML5kLgyOyjlWJ+6PTGc5rp55DBkSHy5EO9JR1Kd/xHX8KyZHgs7Bbu8dY7fcYbqQHCK4OAx9Af0NY1I68xvSnpynH2tv5mqid1QTSzAv5YISONQQqDPOBk9eT1q0k32rXraE8hrjePwBP8hV6/eJXElvGsNvED5YX+PP8RNZXhVheeI7nVpOLWzUwQH/AJ6TN94j12rkfVqwinKR0zkowZu2TncQf+fhmH/fOf5g1pWjkO8meR8qfXpmq2maPf3BeQxfZ0ZiVMvBxzjj8a0rXTLuy8sTiJn3ZHzEqR9fWupHA2jUtHMaqnsSfarNvjzSB2BqiuIm2kkyOcYIxn/61XbcjzyB/dPP4VZmzSHQUtIOlLTEFFFFABRRRQAUUUUAMf8Ah+tUl4jKLwc/Mfarr/w/WqCERqVYnJ5J9zQAOy79gPJ9qJA3ljbxsOaQArIRn5mOcDsPrTsfKG7Dg8dvagAUYIIHfPPfpQ3U/wC43/oJoUAueSUwOPWm7w7HuQjZP4GgCZflgUHgbRikjbBwKYZASpxgAYAp47UDKOoHZfE/3kFc7rEXmxvz2rotUAMyEf3cViX6ZU1x1PiZ3UvhRieDGP8Absrnh44yj/8AfS4/SsfUZ2tPFGqBWIV7qQj8WJ/xrV0WZbPWLlSMNMqnP+6f/r02/wDCl5qWr3l3cXKWcMkzNGuN8jgnOcdAPqc1m/gRumlUbfYzxJPe43PkDpXV+E7KPTNP1CRQCyp5jt6tz/Tj8K5kWsmk3QQzLcQMcCQDBB9xXUaBeQrY6kZQWTYqEDqc5HFOlpNE19YaFKyTzrvXbkjOy9aFD6qPmH/odcxqwyZR7Gut0+FrXw7HHIxZ3LOWY5JyTjJ+mK5LWTtWU/7JpS3KpnTwaelvpdvexRASxqGl2jBdPX+hrYjliRDFIrGFhuEi859QR+Rz71JbR40m1XADeUvXp05B+tV4UCSC13cMPkburL/9auxxRwqbOY1hbvVHlttHtXmlmXywQMJGD/EzdAP8K6Cy09NK06009H3pbRLFvx94qMFvxNaMd2JFYMNkiHa6Hsfb1pWtXkUNICCf4c4wKUYKITqOW5zmvXttbQR2rTIs88iJGpbGQWCk/hn8q7eRMQCIKR8uAf7tc/eaVbXxt7BrRWSSUOflBBK/Nz+A610M78bSN5PUVaM2zD1N1jYRTMNjpsZ1PGD0+hB/QmqOlXlpJHfWF7t8iZxCYnHDMVHH6VvXMZSMEqBu42L3+tZ2kaTBqGqvq19aJvsm8u2QkkA9S5HTPTHpSa1GmrGXF4HN5A1tJdXNpYIf3YUje6/3cMDt+oOMdAK6DT/D9jpsMcFrbJDDEMIo5x68+55PrWucscnk01ulCilsKVSUt2MAAGMVT1PVrfSbctMBI5GfLz0HqaszTrbxNM/3UGSPX2rk7tIb4PJeR+f5r7ioYj+XapqS5diqUOZ3ex0OiXj6lpa3siACViY1x0TsR/npVu3XZebSTxGa5C98UXSQstossgiAVvs6E7fQAAZNdXpjvcQ208wxMYPnHuRk/rRCaegVIOOrNgdKWkpa1MQooooAKKKKACiiigBj9vrVD5QMOdoI+XPrWg/b61nFd4CkcdQDQA5zuG7PUY4psjNtCZwpGM+lGcYViWBHB6UrDemM98kj0oAVW2gDrnAoK7RxgDa2ffg0E4PXn07EdqDnIz/cYY/A0AN2lVzjIqrNuGcZA7e1X1UMoMZwccqajdcghl57ikMwbeDybmaUZIlxnJ9P/wBdNvsCMkVsSWgFpI/8QGRWaYTcSRwqm8u4GM4AXuT+Fc9RanXRlp6GfpGmxWk8eoXSZur1/KtVIz5adS+PXg/gPerl49u0youWWaQRp/tEfeb6dfyNU7jUjFfatqtwR5elxeTboB0LDJP5cfiapXbXS6qEjQmWztVhjjHObiUFT+Q3k/hWfSyNbNu7Luk6Pba9qNxPcI32C2bATOBI3pn264HqK6JdG0uON0gtVhWTBbaSM46U/SNPTSdKhsRtLoMyspyGbualkkAYAjKn7pH8q6YwUUcc6jk9HoZcugRfZVhhunjjjwuXXccfpWFqfw3GowSquutEJFxk227Gf+BCuyZeHQEZK8ZpGYRXVvAT8hQ9e/b/AD9aPZx7Aq1RbMoRadPBpkNq8q3LwRLG8qjbvIAGcc4z161lXAnsbhZ5rS4k4P8Aqoy+TjGeOn/1q6aNDHEUHJZiW+lDErIvJ4NXYhSMfTrcXpj1KWJondcKj+nYketWbmSOFWZ2wACRhvmcjqAD1rQlIfknn+8DyK5rVtIvbne6HfHEB5S79pOepX0YdeeOmKid7aGlNxb94uaRfpeXixllEu3coAI3HuD6Ef0NXr3UbTTY/Nud+WbaqqvJPpnoPxrJ8MafdperqV1GoVlYB5AUduwby+xPzfhj1rent4b6CWC5jDI+VkX09x6H0pw5uXzFU5VPTY5XVfEN7cIUt1SzVuCy/NIB7Men5VqeDVZfC8cju0jzTyyM7HJYlz3riNXN1o2pSabdbpZF+aFgP9ah6MP5H3BrrvD+q2+n+F7C1njlNykeZIlXlWJJwSfrWMJvmfMzoq01yLkR0mahvLu3sIw9zJtLfdjXln+grJl1y6kTEEK2wP8AGx3t+A6VlysFLTzSM8jdWc5Jq3VXQyjRbfvE+palNcj94BDAORGDn8z3rEub3MXPCHgKOp/+tU1y7OhnkOIwMKD3rFeRW+fergHqpz+Fc7k3qdcYpKyLgvriC1ZbeVLdOgY88nviuw8IMsmmI/2hrl8uHlZNm48dBk4HTvXBSQzCBZbi1uY7UHO8xlVJ+pGK9K0VN9lb3At/soMOFhxgAYznHvWtJe8Y4h+6bY6UtJS10nEFFFFABRRRQAUUUUANft9azoxmQuR7LmtF+g+tUFOUOcD0AoARu3PT1oUEgDPLH86a3Kljnd3HelUEfKSBxQA0shXc/c/Kv0zThkfKeyMcnr900yQMSQODj/vmpeOgHADDJPX5aAFVuBng46ipSFmXB4bsarNwo5p8b5AYeuCPQ0rjJFB5icYyMH3rDgfybyMPxh9hPpng1vhlcYfr6jtXP6tGYb6QH/loA4I71lV0SZvR1bRSl0O9je5sEYTGe5WYsegUY6/571v6Zpq2FqzTqj3M0rSSPjJUsMYB+nFVfD+rw3s8lrI+6/hBaTJ++hPBH0yAa1pCXDNHhh3GaqCj8SJqSnflkV5LgwHywwZSOSRyKzvtM0okdHAijzuc8jI7CmSXJ1WR1tDui+69x/CpHBA9T9PTmnzmKK3W3VMRqMBTyKUp9hwh3OdvfF8ep3C2ejPNeXKk5jtug+p6Vq6f5ljYLfavcokxYu0SHIjBxgD8qh26fpiTX0VrFDOeCYkCl/Xp1+tc1NqsfiDUWiklby0b5o1P6f8A16yUmn5nQ4pq2yOks/F1xqOvw2WnWe60ZsTynOceoPQV1MineApJA9awNOaw0yBZl2W67drqf4e+c1rrfRSQpLGCyOPlI71vDbV3OWpa90rIlKEsASPQ1Xmfdc44IUZOT8q0ouS6nZC5xwTuxVXUHeGAfIqBl6A5NUZliC5adxJnAyY8j+f50QXflQTuBli4BH9aq2c8axQqOC77gBz2/wAahL+VNKhIIYkfqKLjsVvGkUaafBeFf30Fwojfvtccg+2cH8Kq20iCAHAyepqbxsxPha6k6+RLBu9gCAa5aDVVNsP3g/OuWrZTudtBXgbtzeoueazHvJriZIYInnmkOI4kGWb/AD6ngd6NK0298Q3JSzwI1P724f7kf+J9h+OK7rS9J0/QIStuPMuHGJbhhl39vYew/wDr0oQc9XsOpUjDRbmNYeEZpFEurzAueTDGcqg9M9z+la8Om6bYXHnwW6I4H3ulWZnkZPkRsEelU57e5kkB8qRjgYAQ4WulRSWhxucpO7ZM160k7fL529Ngjb7uPU1W0PV01bUJHgnWeJUZfMU8MR6e3vVTUNGvNVt20wC5t7eY/wCkzJ8jOndAT0B74+laukaLbaNtisrNYIliKZAwTjpnue9Gtxe7Y26WkpasgKKKKACiiigAooooAa/b61npgEjOR3FaDdvrWdACSwPByTn0oACMyhACSed3oKRWyVDDkE9vT/8AXQWLk7OFKnLf0p2CSAqgKuRz2Hr+NACFSCMt0BLEfy/p+FK5PmbcYGxuPTikUFigXAG7JyP89hSZJmbqcK3P4H/69AClRjnkUiZjJKg89RWmAMClpDuZ+4kgiNwfULWdq9pPdSQlIJM4KvtU4HoR+tbstxDBjzZFTdnG44zUR1C1DbfOGewweevT16dvb1pSSkrMqM3F3Rz8OhPGB5Vs0Td5Bwx/HrT30C5mAine4lgByUeY4b688j2Nbn9o2uyRzIVEZAfKEYycDtUbatbDOA7YGT8uP5/n9KhUoo0deTK32G5jt1ihhjRVGFUEAAVSn0bVJuVe3X6sf8K3LW7W7V2RWUK23nHPAP8AWp6fs0SqsjjpvB2o3ZzcXkBx0UbsfjxVj/hFdQEAhhv7e2A7xQcn9a6mij2UR+3mcoPAkUwT7fqU9yU6ADYP51u2ukW9raJax8Rp0AFWpLiCF40lmjjaVtsYZgC59B6msxr+5FuGluLaF3ICAkdT0B5PXBH0Bq4wS2RnOq5fEy6unRIpVXkAPJ5FMk0m1l/1m9/q1VItSwslzLer5MDCOclcKjcjHT1K+tV11JmCvJemSIuqZhjZyxJZRjC8DcpGT3Ge4quV9jPnj3NKHRLCB1dIm3L0JkY4/WnLpFgpyLZSc55JPP4mqFrq0ELhnmln8+4+zoxxjcCc9T79OvHQ4zW5Q4tbgpKWzKs2m2VxBLBPaxSxTY8xHUEPjpkd6iTQ9IjACaXZqB0xAv8AhV+kqbF3aIVW2s4xGixQJk4UAKM/Sk+22o3fvkJXrg+2azdcvja32nRGON45pCHLnGBlRxyM9c9+nTqRTsbuS8uId0ItJZgytuhcs2M7RyRjClWOeDmtFTk1cxdWKly9TdN/bLjMq/MgcYBPynofpRDfwTyLHGWLEE/dPGK55l1SWFQICblLWF4/3Wwb2bD/AMJAwpIwTx1x3q7btqwvbM/Zv3IJFw2xUOCg24HXhtxPpTdNrqhKsn0ZuU2X7n4H+VOyB3qJ5omJjWVC4BO0MM9PSszYlpaQdKWgAooooAKKKKACiiigBr9B9azXBIxnGc5+laTdvrWaTtTgcsSBnvQAgUluDjPJJ/LNSEo0bPg4HzZ9TTQqYwScn5iO5p5wWwR8vYetADSNsW5sbmOW/wAKD98djsbI9eDzSElmYt98dcD2zj9aRD5khweQGz78UAaY6CiuTHjyF0jMenyfOSGVpApjGQAW9Acjnnimv44lCbxpoVAShkaXKFgMkAgc9vzrX2U+xz/WaXc6ie0iuXQygkJnAzgHp19egrn9Pv0lFo9/HBCl20ixb8p0wFCncd2c8dDwMAYFVj4v1FmmxaW8Yg2iTzGOVJ9geQMHkVH/AMJPey5jiFoNp4CrnZ+tVGlJLVGcsRBtNMtRancXNvuit4ZDwsqrDkCQRSMyn0IYLx2zjvTbae9jSzNqs00LXGzeINjTIduSx24ABZ+u3IGQcjmvNr+seXI0MiswU7UVF5P5VN/ad8JnQai1ziMHzUj2gAEZbHbrj8avlt0RHtL9X/XzOsVFXhVAHsMU6uS+13Xy+ZdS/L8q4Y5Y+pGck8jtjilOXngknMksCk7oxISScfKSM84J/r2rL2bOj2y7HVkgDJIA96ilvLWD/XXMUfGfncDiuN8SSPaeFLu4F99hMbRkXbJvKDzFz8p4Oen41zWja34d1LULxW121la8iC+RKJIF3Dpjcdo+gK/jWFRuDsjaDUldne+I5LFFttSu9StbWzhOySWXkDcyMNpzwcpjPvVK8isLZLdbrWY43nkX7LIkLZMaBiNpB+9hmO4cEdsZzBaF5bS4tbm1imhI8ue1mGSQMdQeCMYII7c4rE1O7sLa0/sHQ9Tjkwi7LUXKs1iBkgpI5zjAAIOcAH7uaTxEoxugeHhKV2dS2o6Ff6PqBW7lmtGucTSRxnAf5TtBx9PzqS2/sezt4oRNKoUR7FkYBjsYuP1bmvH9Q8a6toGpLpGmE2VlaZSJEz+9P8UjE8sWbJya55/FGoNqJup53kkL5JLVj7fENe7saewpXu1qe2+INWsNA8MtrUGnXGo2cNyJJI/P8sx5YYbB+8u/bxz2PSuQf9oMZITwwSOxN9j9PLraj1OHUfhdrd3Pgw3FpMF/3gnH/j1eAIeK1p1XUjeW4nTUHZHs+m/GzVNVupIYdEto9qblBlZjnIGOg9atav8AE3xJbTJa2drp73AUeaNjsNx/hHzdv515t4AdU1yZy6oRCdjvjCtkYJz74rstOs101nvrmJkvWbbBDId2045c55IHb3A61lUnJSsjlnJqTVzp7DWPGVzbSvd6nawXrR5t7dbVSqtjje3JGemOverU134o1G5N1c3cuk6TY2wuJfKKGW4mK7jEDg4VD8pOOffORh6Zeak18AI7ZLMOfMkklZ55fRlAGFyfUk1t62CNB1O4iLee9p5TLngrnOSPUZb8zUOUl1JUmjhvBXiPxBr/AI4jjvtdvTaxszyJ55SPaoLHIGBjiu5hk1X7XeW2oPJJJasVivy5UXELfMuFHy5XlWI6bR61w3wsZP7Qv71oD5McPTG47vqfbPX/AArb8VagviXwhdDSLllmhIkubUnbNGg+8rr1GDj2460Sd3YbfQo63JrM149pYCOGGMAtqN4+/eT2RO+OnIPTtWt8O4vK8UbXl+0TLZuHnMYQyHcDnaOnUD8K53TdQXUdCglOfOtgIpg3Jx/Cc/p+VdB8O2LeMHyc/wCiPj2+ZaI/EiU/eSPWKKSlrsOsKKKKACiiigAooooAa/QfWs0r83zsc+noP8/yrSfoPqKz0G1xv5LZPPYUAO4B37ckjn/CmhtzserEdfSkLeZJsHUdfakYbkwMbs/L70ADMUXbgZzjJ6fjTLeIxyEnJyjfMT046VJKQIyzY5PpnA7miIENgnopznnnH/66APObfcQhO5HZd0cjA7mGTgj6n065qddgd5QxjJUgmMgiNehOeh4x1IqCEjOzeWjG4DYCTtHOVB6D2z61KX2wM0oSQAY2DhmwoAG0j1yM98H2r02eCiby1kTyyDFhTkKwyOeAueeM8g5zg+1P+1W9tpFvZvbCOaA4MiAkysSecAZJbjihiRI+6bzQFJ8/eSJBwNozySSSc8d/oVkgdyZgkkTWc6EORkJKDlRg8k9OPcetSWrrYsgPAWFzG8EiqC6PgkD8Pb0qZg6RlpEwyqRtJ4JA5G73IHt29KY9zPeSLNMdzg/fX5UQMflye3OScn8qVCgRj8oQgqxfAA9s49Rnt1qNepqrdC7H94OrZY7XDAbcN7Z57/5zVld2BwOmeTx7fjz39KowzLcZnjkEhJyGY7uxAz79vyrSi5UlQ2OvI5PHBrNnRDU574jrj4Z6uADtzAOOP+WyfrXhbafCTsa48sjghl5z3+le/wDjy5Wx8A6neNAk6xmL93IMqwMqDPHcZyD6ivGDr+jLbELpAEj9GLZA9Pf14zXFWclLRHVBaHReEfFOtaGbbR9QsY9U08j/AESRnXMS8klXPAAGTgnjFcncXp1XU7/Vbl9y3DMZfn+YjIYj1wflX6Gl1HXvtNq8dnH5MRi2uuM49cH3FUNNZJbhria3Rre1QPIpztbBGFI75OB+fpWaTerNk+iOht9I1TXLBNTv9T07TraNR9mivZCGKdvLjUFgvHHGPTPNZPiLR30Fo7eQM5fDLMeBKCAdy/7Jzx+uDxU0OoSyao1/qjCZ7uMgREABVBBXH91eMDHbIArodE8UaekOqT6/YwXAFt5ls88Z3yzKwCReyEH7o4AGevNZ++paLQ00aOt0WTS9K8FwWWqqWtLW233ce3O4ykEDHfAOTXn+vaLpzazNpVpHGl037y2kg+5IpGVUjscVL4K137V4ptl8Q3mLOUzec85xGWeMqC3bvjnAGa7Sfwxp2oX8jaPHcwXSY3R3EJUOo6PE+SGXGCME8Vmozg9wk1NaHmvheFo9UureaO5EojK+RBAZJHII4xwB7kmuwtozGqs0Rt2ZSWieRZGX0+ZeOfTtTtb0e70jxAl3KHjN1bGK4YcB3Vhgn1yMflTLgqu9FLCSNFkI7SKc4YfQggn6etVOV5XPOrK02X7O6kVnSGcRSsDsdhnyyehx3x2HsK3NOe306L7FBFJHHjJMpz9o3ZJJY/eYnOc888cYrj7K83ToQVIU8ZPGfT8a3Pt8sOqJEiyS6feq0kZyWNpKPvIT/dbPH1HvUy8iLm2TaW1q1tbW6QwudzxpwGJ65qiNRhkvWkk8uS4jXZK5T5ih52FvQjsPbPaq8142SOPKKce7Z/w/nWJI0vmuYEYoxZiDx83+cAewFTFX6CV2UNQSPwrqxvosvY3QJTPzCRScFPqP5iuy+Hvlp40kjiZmjazZ0J4yCVIz79ufT3rkXju57aSzu7A3dnK/meUZRG0b9NytzjI6jHPFdf8ADr7R/wAJXJugt4YjZHcVBLk5UBQf4VUfmeTntvGLunY1im2nY9VpaSlrqOoKKKKACiiigAooooAa/QfUVnnkkd84JrQfoPrWeqhZWI4JGBigBOASfujJyfrQW3Dphffrimtyw9uKe6ZB38r2/wBqgBhAYNnJBzye9Pi3byDxwcD8DTWJCAkDOQCPTNOTAkIA52nOfoaAPN4SnzqI1fEhcRSDc3H95hzjHYemasxNKHWWGSSSZVL7goO1uQxzzuGO+fWqkAJX7OAgSHe+8soJBOGG7+LrwPSpHmjaNyZVDEAAsQWzt4xgfh/OvU5W9kfP8yW7LKLuR4o1J3fKpBBCHG8sMH720E85HbrT/Mge5ZonVGQbxHE+CpHQ8k4/nVd7yzBcKy7c4RAWOBnjJI5HU+tLFq9vFpwsGh3p5xlMwX5+cds4JHIB9MU/ZTeyD2tNbsv28F7cWI1PYqWwcrHGy/vCqnazNngc56/XNPlg+1QGH5V6DcxODj+91JzjkDj5vfjFOuxW8TQR2snl7i3lmTCbiBk4HqRkj3pj+JHknE32UMoBxG0pALE/eO3BOB2zjvXNKpFNps7o0ZtJpfiddNdmedrl4lgwBu2knjqDx7jA/OrtsHU4KlDjOxu1cEfFGoh12pbKUHGYyeueeTjuaYPEesgFY73ysf3I1H9KxdSNtDpjSnfU6X4nhh8LtZJXAzD/AOjk/WvnTzM4z2FezXF9e39t5OoXUl1buBvhlOY2xyMr0OCAfwqe10e7FlHe2tnBDbSMEjddqkksF6Dn7xFdf1HRSlJK5wrMtXGEG7HjEUN1MD5NvLIG/uIT/Ktiy0nVVswv9l3UnmSbypjKg4GF3H0HJr09oLzyp52b91AQC5BG/twCAeD6gVUMjMrHJ5Bqv7Pg4t8xH9q1OZLkt8zgLfw9rMsks9xakFjvCvIo8w/wg89B1xU48Laxc3BmvpLZtxyVaQ/L9MDA/CvRPC2i2/iHUprS7mmijhh8wNCwBJyBzkHjmoYdNtriBJHuktl6mZpVIkGMnC9Vw3y4PXn0NeUkj232OQsPCkFpMWupxcxH70Y4z7fSu90XxQ+jaathZaev2eI/ukeYkRnvjvg+n1rPu7XSre1kMF5LNdf8s1yNv3sHOBzxnuOmehFVbc/K31rpwlKE66UvM48bUlSw8pQdnp+Zo65rk2vrFbXsMMaxyeaoiBBJwRySemCazpIoGCebEMgHYTkHacZ+oO0flW3pmu22neHbzS3jlea5lLo6AbQMKOSTn+H0NRR6/Ekm6W2ABBLeWRnd22+i/wAOOflJFer9Xppv90jwZVpyScqru/w8jHSys4FZoraNSRnOMn/PJ/OrFlpeo3+n3V5aKGtbb/XDdgkgZwB3ODUAkURlQdxx/DzVmxn1yPTrjTrCyumtbvPnBbZmJyMHDY44rjx8IxnFJJaHp5VJyhJt31C20e5uy5imieFCQZ1bKlhjKjvkZqSDw/f3BVVeEM4DKA5PBxgnA6YOfxqf+yfGF6uBZXm0jG0ssQ/IkCpV8EeJ7ti9xHHGzHLGa4DE/XGa889YqR6RHLHGwvQrOqkjAOGIB2Y45xznPce9afgaIweM7q3JyYoJEye+GUU+H4basWDSahawkchowzEH8hW94c8FHQNSN82oNcs0Rj2eVsAyQc5yfSgDrKKKKACiiigAooooAKKKKAI5n8uPdjOCKpMrImHXGTkkf4/Sr7AMpBGQahEW3Ox2X2HI/I0AUFzKG3cgHIUelSzHGI89QefSpmQb/miBI/iTg/lUUtuJ8qJeSPut8poAjUAMpB7EY7elOTm6kIB4Ugn1ODSSK8CglDkYA9B705CAV5G3a3Pr8tAHkaYWMkjIBrduPDT2mnWF/Pejy7+SONVSLJj3jIPUZx6VgRyxsNn3iT90dTWs03iHUbaK1aK8nt4MGFEt8bNowpBAzwK+lqc+nK7dz4+lye9zRbfQdHokskSzGdEt5VLxSEfMVHOSo6HHbPcc1nspR2Q4yjFTj2rQi8OeIJwAum3AXsJGCgfgTVyLwRr8n3o7aEf7cv8AgDUKtCL96aLdCpNe5TZj6Qto/iO2XUTGLIsfOMpwmNpxk/XFaGoXGgprV2LZbb7I3li3aKHciYH7zp6/Q8jt1q4PhzqErt5+qWsYPZFLfzxVyH4ZW4x52rzuP+mcIX+ea+fm05trufVU01CKfZHL2d9a29stlfLJe2iSO2xTtDZ2hWGe4w3XpuqG/v4bxIlS3SDyhyVAG7IGc468g9c9a7uL4c6ImN73s2P70oGfyAq7F4F8OQnK6WHPrJM7fpkipLR5qJE8tcsOlXItbnSyWygSIKuB5iqS5w+8d8fe9unFemx6DpFuvyaZZqB3MQOPzq2gt4hiPy0A7IoFem8dBxScL2PGjltRSbU7Xvt2PKI11ee1W0htLuW3H8KQE55zycc8+tTReHNemUhNKmXION+E/ma9T85D/Ex+goEgPRWOPU1Dx8rNKKVy45XFNOU27Hl6eAfEVwu2SK2hH/TSb/4kGrkfw11FzmbUrSMnrsVn/wAK9F3HPCAU4Fz0wK889Y4WD4Yxqf3+sSv/ANc7cJ/MmtCD4daRD9+a9lz1zIoB/IV1S7ieTTqqMpQd4uzInCM48sldGDF4L0GL/lwD/wC/K5/rV2Lw/o8P+r0uzHuYVJ/M1oY5pcVTqze8mTGhSjtFfcRx28MPEUUaf7igVJ+dFLWZoklsJiilooGJS0UUAFFFFABRRRQAUUUUAFFFFACUmKdSUAMZO46011yMYyDUtGOKAIQhUfKxX26ikMTE/chPqStTelKOtAEUaJEu2Py41HZFxTsg/wAbGgKKUAU7CuNyvox+po47Rin4FGKNA1EDHGMYNGW9adiigBMH1NGMUtLSGMkXchFMEI9KmpKAGeWMdKUKBTqKADGKKKWgBKKWigBKWiigAooooAKKKKACiiigAooooAKKKKAP/9k=</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Waterproof-Hypoallergenic-Breathable-Lighting-Mall/dp/B077MXKFG7/ref=sr_1_18?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-18&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>LEISURE TOWN Queen Mattress Protector 100% Waterproof Mattress Pad Cover Breathable/Hypoallergenic/Vinyl Free Fitted 8”-21” Deep Pocket</t>
+  </si>
+  <si>
+    <t>81 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin XL:$14.90/Queen:$24.90</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71c5GkgJHUL._SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/LEISURE-TOWN-Waterproof-Breathable-Hypoallergenic/dp/B0788GYT6L/ref=sr_1_19?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-19&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>Harmony Dream Mattress Protector Full Size - Premium Waterproof Hypoallergenic Breathable Cover for Mattress - Machine Washable</t>
+  </si>
+  <si>
+    <t>39 customer reviews</t>
+  </si>
+  <si>
+    <t>California King:$29.95/Full:$23.95/King:$28.95/Queen:$25.95</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/81r4s86Q25L._SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Harmony-Dream-Mattress-Protector-Full/dp/B073F9MZJ1/ref=sr_1_20?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-20&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>King Size Luna Premium Hypoallergenic Waterproof Mattress Protector - Made in the USA - Vinyl Free</t>
+  </si>
+  <si>
+    <t>7,715 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin:$29.95/Twin XL:$32.95/Full:$38.95/Queen:$39.95/King:$49.95/California King:$49.95</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/61XnCJslmDL._SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Luna-Hypoallergenic-Waterproof-Mattress-Protector/dp/B002AQPUW0/ref=sr_1_21?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-21&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>The Purple Mattress Protector - Queen</t>
+  </si>
+  <si>
+    <t>3.8 out of 5 stars</t>
+  </si>
+  <si>
+    <t>32 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin:$49.00/Twin XL:$49.00/Full:$54.00/Full XL:$54.00/Queen:$59.00/King:$67.00/California King:$67.00</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/612H3DZH%2BsL._SX450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/The-Purple-Mattress-Protector-Queen/dp/B01N74VK18/ref=sr_1_22?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-22&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>Mattress Protector All Natural Organic Eucalyptus Fiber Top, Hypoallergenic, Breathable, Thin, Quiet, Smooth, No Vinyl, No Odor, Biodegradable Waterproof Fitted Cover, by One's Own - Queen Size</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Eucalyptus-Hypoallergenic-Biodegradable-Ones-Own/dp/B01M68KBG8/ref=sr_1_23?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-23&amp;keywords=mattress+protector</t>
+  </si>
+  <si>
+    <t>King Mattress Protector Premium 100% Waterproof Hypoallergic &amp; Breathable, Vinyl Free, Quilted Mattress Cover Cotton Terry Surface Machine Washable,15 year Warranty SOFTCARE</t>
+  </si>
+  <si>
+    <t>70 customer reviews</t>
+  </si>
+  <si>
+    <t>Twin (39"x75"+14"):$19.90/Twin XL (39"x80"+14"):$19.90/Full (54"x75"+14"):$22.90/Queen (60"x80"+18"):$19.90/King (76"x80"+18"):$23.99/Cal King (72"x84"+18"):$26.90</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71eTF149-yL._SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Protector-Waterproof-Hypoallergic-Breathable-SOFTCARE/dp/B078PBMD69/ref=sr_1_24?s=bedbath&amp;ie=UTF8&amp;qid=1522624327&amp;sr=1-24&amp;keywords=mattress+protector</t>
   </si>
 </sst>
 </file>
@@ -399,7 +744,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,6 +785,472 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" t="s">
+        <v>116</v>
+      </c>
+      <c r="F23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
make headless chrome the default browser
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
   <si>
     <t>Product Name</t>
   </si>
@@ -24,19 +24,19 @@
     <t>Star Rank</t>
   </si>
   <si>
-    <t>[Sponsored]Pillowtop Mattress Pad with Fitted Skirt - Extra Plush Topper Found in Marriott Hotels - Made in the USA, Full</t>
+    <t>[Sponsored]Mattress Pad Cover Queen Size Pillowtop 300TC Down Alternative Mattress Topper with 8-21-Inch Deep Pocket</t>
   </si>
   <si>
     <t>1,1,1</t>
   </si>
   <si>
-    <t>[Sponsored]Bamboo Mattress Pad with Fitted Skirt - Extra Plush Cooling Topper - Hypoallergenic - Made in the USA, California King</t>
+    <t>[Sponsored]Queen Overfilled Mattress Pad Cover 8-21”Deep Pocket-Cooling Mattress Topper Snow Down Alternative</t>
   </si>
   <si>
     <t>1,1,2</t>
   </si>
   <si>
-    <t>[Sponsored]Pillow-Top Premium Mattress Pad - 1.5 Inch Cooling Down Alternative Polygel Filled Microplush Super-Soft Hypoallergenic Topper (Twin XL/Twin Extra Long)</t>
+    <t>[Sponsored]Fairyland Mattress Pad Cover with 300TC 100% Cotton Quilted Down Alternative Filled Mattress Topper,8-21 Inch Deep Pocket (TwinXL)</t>
   </si>
   <si>
     <t>1,1,3</t>
@@ -60,15 +60,15 @@
     <t>1,2,3</t>
   </si>
   <si>
+    <t>Mattress Pad Cover-Cotton Top with Stretches to 18” Deep Pocket Fits Up to 8”-21” Cooling White Bed Topper (Down Alternative, Queen)</t>
+  </si>
+  <si>
+    <t>1,3,1</t>
+  </si>
+  <si>
     <t>Queen Overfilled Mattress Pad Cover 8-21”Deep Pocket-Cooling Mattress Topper Snow Down Alternative</t>
   </si>
   <si>
-    <t>1,3,1</t>
-  </si>
-  <si>
-    <t>Mattress Pad Cover-Cotton Top with Stretches to 18” Deep Pocket Fits Up to 8”-21” Cooling White Bed Topper (Down Alternative, Queen)</t>
-  </si>
-  <si>
     <t>1,3,2</t>
   </si>
   <si>
@@ -84,196 +84,268 @@
     <t>1,4,1</t>
   </si>
   <si>
+    <t>Hypoallergenic Quilted Stretch-to-Fit Mattress Pad By Hanna Kay, 10 Year Warranty-Clyne Collection (Queen)</t>
+  </si>
+  <si>
+    <t>1,4,2</t>
+  </si>
+  <si>
     <t>Queen Mattress Pad Cover 8-21”Deep Pocket - Cooling Mattress Topper Overfilled 300TC Snow Down Alternative</t>
   </si>
   <si>
-    <t>1,4,2</t>
-  </si>
-  <si>
-    <t>Hypoallergenic Quilted Stretch-to-Fit Mattress Pad By Hanna Kay, 10 Year Warranty-Clyne Collection (Queen)</t>
-  </si>
-  <si>
     <t>1,4,3</t>
   </si>
   <si>
+    <t>Premium Mattress Pad (Queen) - Quilted Fitted Mattress Topper Stretches Upto 15 Inches Deep - Plush and Soft Mattress Protector And Cover With Deep Pockets By Utopia Bedding</t>
+  </si>
+  <si>
+    <t>1,5,1</t>
+  </si>
+  <si>
+    <t>INGALIK Hotel Luxury Collection Quilted Fitted Mattress Topper Down Alternative Overfilled Mattress Pad Bed Cover Stretches up to 21 Inches Deep by (Queen 60x80x18inch)</t>
+  </si>
+  <si>
+    <t>1,5,2</t>
+  </si>
+  <si>
+    <t>Beckham Hotel Collection 1500 Series Microfiber Mattress Pad - Quilted, Hypoallergnic, and Water-Resistant - King</t>
+  </si>
+  <si>
+    <t>1,5,3</t>
+  </si>
+  <si>
+    <t>Mattress Pad Cover with 18" Deep Pocket 300TC Cotton Down Mattress Topper By HYPNOS Mattress Topper Hypoallergenic Quilted Stretch-to-Fit,King</t>
+  </si>
+  <si>
+    <t>1,6,1</t>
+  </si>
+  <si>
+    <t>Maevis Mattress Pad Cover 100% 300TC Cotton with 8-21 Inch Deep Pocket White Overfilled Bed Mattress Topper (Down Alternative, Twin XL)</t>
+  </si>
+  <si>
+    <t>1,6,2</t>
+  </si>
+  <si>
+    <t>Sleep Restoration Fitted Microfiber Mattress Pad Cover - Plush Quilted Luxurious Mattress Topper - Queen</t>
+  </si>
+  <si>
+    <t>1,6,3</t>
+  </si>
+  <si>
+    <t>Mattress Pad Cover (King Size)- Cooling Mattress Topper with Thick Cotton 8-21-Inch Deep Pocket - Quilted Fitted Pillowtop by Sonoro Kate</t>
+  </si>
+  <si>
+    <t>1,7,1</t>
+  </si>
+  <si>
+    <t>Mattress Pad Cover with 18” Deep Pocket Overfilled 100% 300TC Cotton White Bed Topper By WarmHarbor Mattress Topper (Down Alternative, Full)</t>
+  </si>
+  <si>
+    <t>1,7,2</t>
+  </si>
+  <si>
+    <t>Pillowtop Mattress Pad with Fitted Skirt - Extra Plush Topper Found in Marriott Hotels - Made in the USA, Queen</t>
+  </si>
+  <si>
+    <t>1,7,3</t>
+  </si>
+  <si>
+    <t>Fairyland Mattress Pad Cover with 300TC 100% Cotton Quilted Down Alternative Filled Mattress Topper,8-21 Inch Deep Pocket (TwinXL)</t>
+  </si>
+  <si>
+    <t>1,8,1</t>
+  </si>
+  <si>
+    <t>Pillowtop Mattress Pad Cover Queen Size - Hypoallergenic - Cotton Down Alternative Filled Mattress Topper</t>
+  </si>
+  <si>
+    <t>1,8,2</t>
+  </si>
+  <si>
+    <t>Bamboo Overfilled Pillow Top Mattress Pad | Superb Temperature Regulation | Made in the USA, King</t>
+  </si>
+  <si>
+    <t>1,8,3</t>
+  </si>
+  <si>
+    <t>Mattress Pad Full Size with 24 inch Deep Pocket Microplush Mattress Topper with Fitted Skirt Quilted Stretch Pillow Top by Naluka（54”x75”)</t>
+  </si>
+  <si>
+    <t>1,9,1</t>
+  </si>
+  <si>
+    <t>Luxurious - Fitted Down Alternative Mattress Pad - 100% Cotton Top Mattress Topper, 300 Thread Count - Mattress Cover Stretches Up to 16 - Full Size (54x75")</t>
+  </si>
+  <si>
+    <t>1,9,2</t>
+  </si>
+  <si>
+    <t>Twin XL Mattress Pad - 300TC Down Alternative Pillow Top Mattress Topper,Quilted Deep Pocket Fitted Mattress Cover (8"-21")</t>
+  </si>
+  <si>
+    <t>1,9,3</t>
+  </si>
+  <si>
+    <t>Mattress Pad King Size 400TC Cotton Top 3M Water Resistant Hypoallergenic-71oz Down Alternative Filling Pillowtop Mattress Topper Cover-Fitted Quilted 8-21 Inch Deep Pocket</t>
+  </si>
+  <si>
+    <t>1,10,1</t>
+  </si>
+  <si>
+    <t>Mattress Pad Cover, Microfiber, Soft, Hypoallergenic, Mattress Topper with Deep Pocket(Queen,Superior)</t>
+  </si>
+  <si>
+    <t>1,10,2</t>
+  </si>
+  <si>
+    <t>Rayon from Bamboo Extra Thick Mattress Pad with Fitted Skirt - Extra Plush Cooling Topper - Hypoallergenic - Proudly Made in the USA, Twin XL</t>
+  </si>
+  <si>
+    <t>1,10,3</t>
+  </si>
+  <si>
+    <t>Amazon recommendation</t>
+  </si>
+  <si>
+    <t>1,11,1</t>
+  </si>
+  <si>
+    <t>Mattress Pad Full Size Hypoallergenic - Antibacterial, Breathable - Ultra Soft Quilted Mattress Protector, Fitted Sheet Mattress Cover White by Bedsure</t>
+  </si>
+  <si>
+    <t>1,11,2</t>
+  </si>
+  <si>
+    <t>Quilted Fitted Mattress Pad (King)-Mattress Cover Stretches up 8-21" Deep Pocket Down Alternative Filling Mattress Topper</t>
+  </si>
+  <si>
+    <t>1,11,3</t>
+  </si>
+  <si>
+    <t>Naturepedic Organic Waterproof Fitted Stretch Knit Protector Pad - Twin</t>
+  </si>
+  <si>
+    <t>1,12,1</t>
+  </si>
+  <si>
+    <t>Pillow-Top Premium Mattress Pad - 1.5 Inch Cooling Down Alternative Polygel Filled Microplush Super-Soft Hypoallergenic Topper (Twin XL/Twin Extra Long)</t>
+  </si>
+  <si>
+    <t>1,12,2</t>
+  </si>
+  <si>
+    <t>SleepJoy 3" ViscO2 Ventilated Memory Foam Mattress Topper, Queen</t>
+  </si>
+  <si>
+    <t>1,12,3</t>
+  </si>
+  <si>
+    <t>Sleep Philosophy All Natural Cotton Filled Mattress Pad, Queen</t>
+  </si>
+  <si>
+    <t>1,13,1</t>
+  </si>
+  <si>
+    <t>AmazonBasics Hypoallergenic Quilted Mattress Topper, 18" Deep, Full</t>
+  </si>
+  <si>
+    <t>1,13,2</t>
+  </si>
+  <si>
+    <t>The Grand Fitted Quilted Mattress Pad Cover Hypoallergenic (Stretches to 18" Deep - Queen - 60x80") Queen Size Mattress Protector</t>
+  </si>
+  <si>
+    <t>1,13,3</t>
+  </si>
+  <si>
+    <t>Queen Fitted Quilted Mattress Pad Cover 8-21”Deep Pocket-Down Alternative Mattress Topper</t>
+  </si>
+  <si>
+    <t>1,14,1</t>
+  </si>
+  <si>
+    <t>Micropuff Down Alternative Mattress Pad - White Quilted Fitted Mattress Topper (Twin Size - 39"x75") Microfiber Mattress Cover Stretches up to 15"</t>
+  </si>
+  <si>
+    <t>1,14,2</t>
+  </si>
+  <si>
+    <t>Bamboo Mattress Pad with Fitted Skirt - Extra Plush Cooling Topper - Hypoallergenic - Made in the USA, Full</t>
+  </si>
+  <si>
+    <t>1,14,3</t>
+  </si>
+  <si>
+    <t>Hospitology Heavenly Microfiber Goose Down Alternative Overstuffed Hypoallergenic Mattress Pad / Topper, 54-Inch by 75-Inch, Full/Double</t>
+  </si>
+  <si>
+    <t>1,15,1</t>
+  </si>
+  <si>
+    <t>Shilucheng Mattress Pad Queen Size Ultra Soft Rayon Derived from Plush - 8-21-Inch Deep Pocket Premium Hypoallergenic Mattress Topper</t>
+  </si>
+  <si>
+    <t>1,15,2</t>
+  </si>
+  <si>
+    <t>Happsy Organic Mattress Protector Pad - Twin</t>
+  </si>
+  <si>
+    <t>1,15,3</t>
+  </si>
+  <si>
+    <t>Merous Queen Size Cotton Mattress Pad Down Alternative Mattress Cover - Hypoallergenic Fitted Quilted Mattress Topper - Stretches up to 18 Inches Deep</t>
+  </si>
+  <si>
+    <t>1,16,1</t>
+  </si>
+  <si>
+    <t>Superior Queen Size Premium 100% Waterproof Mattress Protector Pad - 100% Cotton Terry Surface, Hypoallergenic, Deep Pocket Skirt Fits Up to 22" Mattress, 15-Year Warranty</t>
+  </si>
+  <si>
+    <t>1,16,2</t>
+  </si>
+  <si>
+    <t>Red Nomad - Queen Size 2 Inch Thick, Ultra Premium Visco Elastic Memory Foam Mattress Pad Bed Topper - Made in the USA</t>
+  </si>
+  <si>
+    <t>1,16,3</t>
+  </si>
+  <si>
+    <t>RV Mattress Pad - Extra Plush Topper with Fitted Skirt - Found in Marriott Hotels - Made in the USA - Hypoallergenic - Mattress Cover for RV, Camper - Short Queen</t>
+  </si>
+  <si>
+    <t>1,17,1</t>
+  </si>
+  <si>
+    <t>Allrange 300TC Cool Tencel Hypoallergenic Quilted Mattress Pad, Stretch-up-to 22", Fitted Tencel Polyester Fill, Silky Cotton Tencel Cover,OEKO-TEX Certified, Queen</t>
+  </si>
+  <si>
+    <t>1,17,2</t>
+  </si>
+  <si>
+    <t>Pressure Relief Mattress Pad with Fitted Skirt |Bedsore Prevention Mattress Pads | Hypoallergenic Mattress Topper | Made in the USA, Queen</t>
+  </si>
+  <si>
+    <t>1,17,3</t>
+  </si>
+  <si>
+    <t>[Sponsored]Queen Mattress Pad Cover 8-21”Deep Pocket - Cooling Mattress Topper Overfilled 300TC Snow Down Alternative</t>
+  </si>
+  <si>
+    <t>1,18,1</t>
+  </si>
+  <si>
     <t>[Sponsored]Bamboo Overfilled and ExtraThick 1-Piece Pillow Top Mattress Pad, Twin XL</t>
   </si>
   <si>
-    <t>1,5,1</t>
-  </si>
-  <si>
-    <t>[Sponsored]Mattress Pad King Size 400TC Cotton Top 3M Water Resistant Hypoallergenic-71oz Down Alternative Filling Pillowtop Mattress Topper Cover-Fitted Quilted 8-21 Inch Deep Pocket</t>
-  </si>
-  <si>
-    <t>1,5,2</t>
-  </si>
-  <si>
-    <t>[Sponsored]Bamboo Overfilled Pillow Top Mattress Pad | Superb Temperature Regulation | Made in the USA, California King</t>
-  </si>
-  <si>
-    <t>1,5,3</t>
-  </si>
-  <si>
-    <t>Premium Mattress Pad (Queen) - Quilted Fitted Mattress Topper Stretches Upto 15 Inches Deep - Plush and Soft Mattress Protector And Cover With Deep Pockets By Utopia Bedding</t>
-  </si>
-  <si>
-    <t>1,6,1</t>
-  </si>
-  <si>
-    <t>INGALIK Hotel Luxury Collection Quilted Fitted Mattress Topper Down Alternative Overfilled Mattress Pad Bed Cover Stretches up to 21 Inches Deep by (Queen 60x80x18inch)</t>
-  </si>
-  <si>
-    <t>1,6,2</t>
-  </si>
-  <si>
-    <t>Beckham Hotel Collection 1500 Series Microfiber Mattress Pad - Quilted, Hypoallergnic, and Water-Resistant - King</t>
-  </si>
-  <si>
-    <t>1,6,3</t>
-  </si>
-  <si>
-    <t>Mattress Pad Cover (King Size)- Cooling Mattress Topper with Thick Cotton 8-21-Inch Deep Pocket - Quilted Fitted Pillowtop by Sonoro Kate</t>
-  </si>
-  <si>
-    <t>1,7,1</t>
-  </si>
-  <si>
-    <t>Mattress Pad Cover with 18" Deep Pocket 300TC Cotton Down Mattress Topper By HYPNOS Mattress Topper Hypoallergenic Quilted Stretch-to-Fit,King</t>
-  </si>
-  <si>
-    <t>1,7,2</t>
-  </si>
-  <si>
-    <t>Maevis Mattress Pad Cover 100% 300TC Cotton with 8-21 Inch Deep Pocket White Overfilled Bed Mattress Topper (Down Alternative, Twin XL)</t>
-  </si>
-  <si>
-    <t>1,7,3</t>
-  </si>
-  <si>
-    <t>Sleep Restoration Fitted Microfiber Mattress Pad Cover - Plush Quilted Luxurious Mattress Topper - Queen</t>
-  </si>
-  <si>
-    <t>1,8,1</t>
-  </si>
-  <si>
-    <t>Pillowtop Mattress Pad with Fitted Skirt - Extra Plush Topper Found in Marriott Hotels - Made in the USA, Queen</t>
-  </si>
-  <si>
-    <t>1,8,2</t>
-  </si>
-  <si>
-    <t>Fairyland Mattress Pad Cover with 300TC 100% Cotton Quilted Down Alternative Filled Mattress Topper,8-21 Inch Deep Pocket (TwinXL)</t>
-  </si>
-  <si>
-    <t>1,8,3</t>
-  </si>
-  <si>
-    <t>Pillowtop Mattress Pad Cover Queen Size - Hypoallergenic - Cotton Down Alternative Filled Mattress Topper</t>
-  </si>
-  <si>
-    <t>1,9,1</t>
-  </si>
-  <si>
-    <t>Bamboo Overfilled Pillow Top Mattress Pad | Superb Temperature Regulation | Made in the USA, King</t>
-  </si>
-  <si>
-    <t>1,9,2</t>
-  </si>
-  <si>
-    <t>Mattress Pad Full Size with 24 inch Deep Pocket Microplush Mattress Topper with Fitted Skirt Quilted Stretch Pillow Top by Naluka（54”x75”)</t>
-  </si>
-  <si>
-    <t>1,9,3</t>
-  </si>
-  <si>
-    <t>Luxurious - Fitted Down Alternative Mattress Pad - 100% Cotton Top Mattress Topper, 300 Thread Count - Mattress Cover Stretches Up to 16 - Full Size (54x75")</t>
-  </si>
-  <si>
-    <t>1,10,1</t>
-  </si>
-  <si>
-    <t>Mattress Pad Cover Twin Size Mattress Topper with 18” Deep Pocket Overfilled 100% 300TC Cotton White Bed Topper (Down Alternative)</t>
-  </si>
-  <si>
-    <t>1,10,2</t>
-  </si>
-  <si>
-    <t>Mattress Pad King Size 400TC Cotton Top 3M Water Resistant Hypoallergenic-71oz Down Alternative Filling Pillowtop Mattress Topper Cover-Fitted Quilted 8-21 Inch Deep Pocket</t>
-  </si>
-  <si>
-    <t>1,10,3</t>
-  </si>
-  <si>
-    <t>Twin XL Mattress Pad - 300TC Down Alternative Pillow Top Mattress Topper,Quilted Deep Pocket Fitted Mattress Cover (8"-21")</t>
-  </si>
-  <si>
-    <t>1,11,1</t>
-  </si>
-  <si>
-    <t>Quilted Fitted Mattress Pad (King)-Mattress Cover Stretches up 8-21" Deep Pocket Down Alternative Filling Mattress Topper</t>
-  </si>
-  <si>
-    <t>1,11,2</t>
-  </si>
-  <si>
-    <t>Mattress Pad Cover, Microfiber, Soft, Hypoallergenic, Mattress Topper with Deep Pocket(Queen,Superior)</t>
-  </si>
-  <si>
-    <t>1,11,3</t>
-  </si>
-  <si>
-    <t>Amazon recommendation</t>
-  </si>
-  <si>
-    <t>1,12,1</t>
-  </si>
-  <si>
-    <t>Mattress Pad Full Size Hypoallergenic - Antibacterial, Breathable - Ultra Soft Quilted Mattress Protector, Fitted Sheet Mattress Cover White by Bedsure</t>
-  </si>
-  <si>
-    <t>1,12,2</t>
-  </si>
-  <si>
-    <t>Rayon from Bamboo Extra Thick Mattress Pad with Fitted Skirt - Extra Plush Cooling Topper - Hypoallergenic - Proudly Made in the USA, Twin XL</t>
-  </si>
-  <si>
-    <t>1,12,3</t>
-  </si>
-  <si>
-    <t>Naturepedic Organic Waterproof Fitted Stretch Knit Protector Pad - Twin</t>
-  </si>
-  <si>
-    <t>1,13,1</t>
-  </si>
-  <si>
-    <t>Pillow-Top Premium Mattress Pad - 1.5 Inch Cooling Down Alternative Polygel Filled Microplush Super-Soft Hypoallergenic Topper (Twin XL/Twin Extra Long)</t>
-  </si>
-  <si>
-    <t>1,13,2</t>
-  </si>
-  <si>
-    <t>SleepJoy 3" ViscO2 Ventilated Memory Foam Mattress Topper, Queen</t>
-  </si>
-  <si>
-    <t>1,13,3</t>
-  </si>
-  <si>
-    <t>Sleep Philosophy All Natural Cotton Filled Mattress Pad, Queen</t>
-  </si>
-  <si>
-    <t>1,14,1</t>
-  </si>
-  <si>
-    <t>AmazonBasics Hypoallergenic Quilted Mattress Topper, 18" Deep, Full</t>
-  </si>
-  <si>
-    <t>1,14,2</t>
-  </si>
-  <si>
-    <t>The Grand Fitted Quilted Mattress Pad Cover Hypoallergenic (Stretches to 18" Deep - Queen - 60x80") Queen Size Mattress Protector</t>
-  </si>
-  <si>
-    <t>1,14,3</t>
+    <t>1,18,2</t>
+  </si>
+  <si>
+    <t>[Sponsored]Pillowtop Mattress Pad with Fitted Skirt - Extra Plush Topper Found in Marriott Hotels - Made in the USA, Twin XL</t>
+  </si>
+  <si>
+    <t>1,18,3</t>
   </si>
 </sst>
 </file>
@@ -627,7 +699,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -979,6 +1051,102 @@
         <v>85</v>
       </c>
     </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>